<commit_message>
Initial update to fuels/PoFDCtAE with EU data and US assumptions/calculation methodology
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\Dropbox (Energy InNovation)\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190E0567-D228-475F-AE92-CB99F12E58B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80BA74C-9054-4E84-AED9-CE504ED44E4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1065" windowWidth="23535" windowHeight="16185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6000" yWindow="-16935" windowWidth="15585" windowHeight="13515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="101">
   <si>
     <t>PoFDCtAE Percentage of Fuel Demand Change that Alters Exports</t>
   </si>
@@ -232,9 +232,6 @@
     <t>exports of petroleum gasoline, 50% of the amount results in increased exports</t>
   </si>
   <si>
-    <t>of cruide oil, and 25% results in reduced production of both fuels.  You would</t>
-  </si>
-  <si>
     <t>enter 0.25 in the (petroleum gasoline to petroleum gasoline) cell and 0.5 in the</t>
   </si>
   <si>
@@ -335,6 +332,12 @@
   </si>
   <si>
     <t>For fuels other than crude oil and petroleum products, we use settings calculated as (present</t>
+  </si>
+  <si>
+    <t>of crude oil, and 25% results in reduced production of both fuels.  You would</t>
+  </si>
+  <si>
+    <t>The EU version of this variable currently follows US assumptions and calculation methodology.</t>
   </si>
 </sst>
 </file>
@@ -434,7 +437,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -491,9 +494,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -507,6 +507,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -788,328 +799,338 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H74"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="87.5703125" customWidth="1"/>
+    <col min="2" max="2" width="87.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="2">
         <v>2018</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="26" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B12" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B13" s="26" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="37" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A38" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A49" s="31" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="32" t="s">
+      <c r="B49" s="32"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="33"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A59" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A65" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="15"/>
-      <c r="G57" s="15"/>
-      <c r="H57" s="15"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1129,59 +1150,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="44.140625" customWidth="1"/>
-    <col min="2" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="100.7109375" customWidth="1"/>
+    <col min="1" max="1" width="44.1328125" customWidth="1"/>
+    <col min="2" max="5" width="15.3984375" customWidth="1"/>
+    <col min="6" max="6" width="12.86328125" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="100.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="16"/>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="17"/>
-      <c r="H2" s="29" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" s="28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="D3" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="E3" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="F3" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="21" t="s">
-        <v>76</v>
-      </c>
       <c r="H3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>32</v>
       </c>
@@ -1191,405 +1214,405 @@
       <c r="E4" s="22"/>
       <c r="F4" s="23"/>
       <c r="H4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="24">
-        <v>1.2994850819999496E+16</v>
-      </c>
-      <c r="C5" s="24">
-        <v>121838241144116.98</v>
-      </c>
-      <c r="D5" s="24">
-        <v>1908500328228990.3</v>
-      </c>
-      <c r="E5" s="22">
-        <f t="shared" ref="E5:E24" si="0">B5+C5-D5</f>
-        <v>1.1208188732914622E+16</v>
+      <c r="B5" s="33">
+        <v>1769370385808722.5</v>
+      </c>
+      <c r="C5" s="33">
+        <v>4304727594014679</v>
+      </c>
+      <c r="D5" s="33">
+        <v>530234220881090.13</v>
+      </c>
+      <c r="E5" s="34">
+        <f>B5+C5-D5</f>
+        <v>5543863758942312</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
-      </c>
-      <c r="G5" s="30"/>
+        <v>76</v>
+      </c>
+      <c r="G5" s="29"/>
       <c r="H5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="24">
-        <v>3.3449389999999996E+16</v>
-      </c>
-      <c r="C6" s="24">
-        <v>2724850000000000</v>
-      </c>
-      <c r="D6" s="24">
-        <v>5184905000000000</v>
-      </c>
-      <c r="E6" s="22">
+      <c r="B6" s="33">
+        <v>2663650455112149.5</v>
+      </c>
+      <c r="C6" s="33">
+        <v>1.396792574668349E+16</v>
+      </c>
+      <c r="D6" s="33">
+        <v>3443870796960235.5</v>
+      </c>
+      <c r="E6" s="34">
+        <f t="shared" ref="E6:E24" si="0">B6+C6-D6</f>
+        <v>1.3187705404835404E+16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" s="29"/>
+      <c r="H6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="33">
+        <v>7762103858922054</v>
+      </c>
+      <c r="C7" s="33">
+        <v>8804296582606409</v>
+      </c>
+      <c r="D7" s="33">
+        <v>0</v>
+      </c>
+      <c r="E7" s="34">
         <f t="shared" si="0"/>
-        <v>3.0989335E+16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>77</v>
-      </c>
-      <c r="G6" s="30"/>
-      <c r="H6" t="s">
+        <v>1.6566400441528464E+16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" s="29"/>
+      <c r="H7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="24">
-        <v>534894468127151.31</v>
-      </c>
-      <c r="C7" s="24">
-        <v>7200000000000000</v>
-      </c>
-      <c r="D7" s="24">
-        <v>0</v>
-      </c>
-      <c r="E7" s="22">
-        <f t="shared" si="0"/>
-        <v>7734894468127151</v>
-      </c>
-      <c r="F7" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="30"/>
-      <c r="H7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
       <c r="E8" s="22"/>
       <c r="F8" s="23"/>
-      <c r="G8" s="30"/>
+      <c r="G8" s="29"/>
       <c r="H8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="22"/>
       <c r="F9" s="23"/>
-      <c r="G9" s="30"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="29"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
       <c r="E10" s="22"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="30"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="29"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="24">
-        <v>127054236057268.86</v>
-      </c>
-      <c r="C11" s="24">
-        <v>3835846580378.2954</v>
-      </c>
-      <c r="D11" s="24">
-        <v>86443847182000</v>
-      </c>
-      <c r="E11" s="22">
+      <c r="B11" s="33">
+        <v>4165397947498852.5</v>
+      </c>
+      <c r="C11" s="33">
+        <v>312642855049688.31</v>
+      </c>
+      <c r="D11" s="33">
+        <v>181192072936495.97</v>
+      </c>
+      <c r="E11" s="34">
         <f t="shared" si="0"/>
-        <v>44446235455647.156</v>
+        <v>4296848729612045</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
-      </c>
-      <c r="G11" s="30"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="29"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="24">
-        <v>2.345837516236748E+16</v>
-      </c>
-      <c r="C12" s="24">
-        <v>65450425688886.055</v>
-      </c>
-      <c r="D12" s="24">
-        <v>1712687718894354.5</v>
-      </c>
-      <c r="E12" s="22">
+      <c r="B12" s="35">
+        <v>4199805007475681</v>
+      </c>
+      <c r="C12" s="33">
+        <v>1013941160881174.4</v>
+      </c>
+      <c r="D12" s="33">
+        <v>2988025433128846.5</v>
+      </c>
+      <c r="E12" s="34">
         <f t="shared" si="0"/>
-        <v>2.1811137869162012E+16</v>
+        <v>2225720735228008.5</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
-      </c>
-      <c r="G12" s="30"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="29"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A13" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="24">
-        <v>1.3635229972917368E+16</v>
-      </c>
-      <c r="C13" s="24">
-        <v>351737454255556.31</v>
-      </c>
-      <c r="D13" s="24">
-        <v>3637018944597630</v>
-      </c>
-      <c r="E13" s="22">
+      <c r="B13" s="35">
+        <v>9413120341769230</v>
+      </c>
+      <c r="C13" s="33">
+        <v>4830704037462619</v>
+      </c>
+      <c r="D13" s="33">
+        <v>4339347553620890.5</v>
+      </c>
+      <c r="E13" s="34">
         <f t="shared" si="0"/>
-        <v>1.0349948482575294E+16</v>
+        <v>9904476825610958</v>
       </c>
       <c r="F13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G13" s="30"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="G13" s="29"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="24">
-        <v>1561489169872463.5</v>
-      </c>
-      <c r="C14" s="24">
-        <v>8008300000911.835</v>
-      </c>
-      <c r="D14" s="24">
-        <v>163819887068608</v>
-      </c>
-      <c r="E14" s="22">
+      <c r="B14" s="33">
+        <v>89807897624285.297</v>
+      </c>
+      <c r="C14" s="33">
+        <v>50292782953843.539</v>
+      </c>
+      <c r="D14" s="33">
+        <v>41931207613454.992</v>
+      </c>
+      <c r="E14" s="34">
         <f t="shared" si="0"/>
-        <v>1405677582804767.3</v>
+        <v>98169472964673.844</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
-      </c>
-      <c r="G14" s="30"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="G14" s="29"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="24">
-        <v>209619113794859.22</v>
-      </c>
-      <c r="C15" s="24">
-        <v>81719279513151.391</v>
-      </c>
-      <c r="D15" s="24">
-        <v>14787150681592.84</v>
-      </c>
-      <c r="E15" s="22">
+      <c r="B15" s="33">
+        <v>470056326182592.56</v>
+      </c>
+      <c r="C15" s="33">
+        <v>252654197726164</v>
+      </c>
+      <c r="D15" s="33">
+        <v>250690991707395.94</v>
+      </c>
+      <c r="E15" s="34">
         <f t="shared" si="0"/>
-        <v>276551242626417.78</v>
+        <v>472019532201360.56</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="30"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="29"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A16" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="24">
-        <v>4515477159886859</v>
-      </c>
-      <c r="C16" s="24">
-        <v>371817123993646.19</v>
-      </c>
-      <c r="D16" s="24">
-        <v>487532159271959.88</v>
-      </c>
-      <c r="E16" s="22">
+      <c r="B16" s="35">
+        <v>1242913561157512.5</v>
+      </c>
+      <c r="C16" s="33">
+        <v>1046968038949733</v>
+      </c>
+      <c r="D16" s="33">
+        <v>631602422132630.75</v>
+      </c>
+      <c r="E16" s="34">
         <f t="shared" si="0"/>
-        <v>4399762124608545</v>
+        <v>1658279177974614.8</v>
       </c>
       <c r="F16" t="s">
-        <v>77</v>
-      </c>
-      <c r="G16" s="30"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="G16" s="29"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="22"/>
       <c r="F17" s="23"/>
-      <c r="G17" s="30"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="29"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
       <c r="E18" s="22"/>
       <c r="F18" s="23"/>
-      <c r="G18" s="30"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="29"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="24">
-        <v>859050369312946.75</v>
-      </c>
-      <c r="C19" s="24">
-        <v>0</v>
-      </c>
-      <c r="D19" s="24">
-        <v>0</v>
-      </c>
-      <c r="E19" s="22">
+      <c r="B19" s="33">
+        <v>3160571929646474.5</v>
+      </c>
+      <c r="C19" s="33">
+        <v>38203004039936.016</v>
+      </c>
+      <c r="D19" s="33">
+        <v>51675019729629.898</v>
+      </c>
+      <c r="E19" s="34">
         <f t="shared" si="0"/>
-        <v>859050369312946.75</v>
+        <v>3147099913956780.5</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
-      </c>
-      <c r="G19" s="30"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="G19" s="29"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="24">
-        <v>2.4934676413517276E+16</v>
-      </c>
-      <c r="C20" s="24">
-        <v>1.4838296942851536E+16</v>
-      </c>
-      <c r="D20" s="24">
-        <v>2994708229987662</v>
-      </c>
-      <c r="E20" s="22">
+      <c r="B20" s="33">
+        <v>875407792588829.88</v>
+      </c>
+      <c r="C20" s="33">
+        <v>2.0931542682938876E+16</v>
+      </c>
+      <c r="D20" s="33">
+        <v>242821039629142.72</v>
+      </c>
+      <c r="E20" s="34">
         <f t="shared" si="0"/>
-        <v>3.6778265126381152E+16</v>
+        <v>2.156412943589856E+16</v>
       </c>
       <c r="F20" t="s">
-        <v>77</v>
-      </c>
-      <c r="G20" s="30"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="29"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="24">
-        <v>1250687800589910.5</v>
-      </c>
-      <c r="C21" s="24">
-        <v>476589424280788.31</v>
-      </c>
-      <c r="D21" s="24">
-        <v>873930050846522.25</v>
-      </c>
-      <c r="E21" s="22">
+      <c r="B21" s="35">
+        <v>2796362077584358.5</v>
+      </c>
+      <c r="C21" s="33">
+        <v>1705325640848346.3</v>
+      </c>
+      <c r="D21" s="33">
+        <v>2247701157347284.3</v>
+      </c>
+      <c r="E21" s="34">
         <f t="shared" si="0"/>
-        <v>853347174024176.5</v>
+        <v>2253986561085421</v>
       </c>
       <c r="F21" t="s">
-        <v>77</v>
-      </c>
-      <c r="G21" s="30"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="29"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="24">
-        <v>4084904971604980.5</v>
-      </c>
-      <c r="C22" s="24">
-        <v>243930593817797.94</v>
-      </c>
-      <c r="D22" s="24">
-        <v>1827886456100663</v>
-      </c>
-      <c r="E22" s="22">
+      <c r="B22" s="35">
+        <v>629613892336042.38</v>
+      </c>
+      <c r="C22" s="33">
+        <v>868822141238955.25</v>
+      </c>
+      <c r="D22" s="33">
+        <v>345705414641558.38</v>
+      </c>
+      <c r="E22" s="34">
         <f t="shared" si="0"/>
-        <v>2500949109322115.5</v>
+        <v>1152730618933439</v>
       </c>
       <c r="F22" t="s">
-        <v>77</v>
-      </c>
-      <c r="G22" s="30"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="G22" s="29"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="24">
-        <v>1730154785433083.3</v>
-      </c>
-      <c r="C23" s="24">
-        <v>0</v>
-      </c>
-      <c r="D23" s="24">
-        <v>0</v>
-      </c>
-      <c r="E23" s="22">
+      <c r="B23" s="36">
+        <v>878812251216380.5</v>
+      </c>
+      <c r="C23" s="33">
+        <v>37448814583497.266</v>
+      </c>
+      <c r="D23" s="33">
+        <v>3084196909499.5342</v>
+      </c>
+      <c r="E23" s="34">
         <f t="shared" si="0"/>
-        <v>1730154785433083.3</v>
+        <v>913176868890378.25</v>
       </c>
       <c r="F23" t="s">
-        <v>77</v>
-      </c>
-      <c r="G23" s="30"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="G23" s="29"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="24">
-        <v>8746500000000000</v>
-      </c>
-      <c r="C24" s="24">
-        <v>0</v>
-      </c>
-      <c r="D24" s="24">
-        <v>0</v>
-      </c>
-      <c r="E24" s="22">
+      <c r="B24" s="36">
+        <v>1290868995.2225955</v>
+      </c>
+      <c r="C24" s="33">
+        <v>0</v>
+      </c>
+      <c r="D24" s="33">
+        <v>0</v>
+      </c>
+      <c r="E24" s="34">
         <f t="shared" si="0"/>
-        <v>8746500000000000</v>
+        <v>1290868995.2225955</v>
       </c>
       <c r="F24" t="s">
-        <v>77</v>
-      </c>
-      <c r="G24" s="30"/>
+        <v>76</v>
+      </c>
+      <c r="G24" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1603,22 +1626,22 @@
   </sheetPr>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" customWidth="1"/>
-    <col min="2" max="22" width="16.5703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="36.73046875" customWidth="1"/>
+    <col min="2" max="22" width="16.59765625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>32</v>
@@ -1684,7 +1707,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
@@ -1752,16 +1775,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="30">
         <f>'Data from BFPIaE'!D5/'Data from BFPIaE'!B5</f>
-        <v>0.14686588977933832</v>
+        <v>0.29967395472075625</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
@@ -1821,7 +1844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>34</v>
       </c>
@@ -1831,9 +1854,9 @@
       <c r="C4" s="8">
         <v>0</v>
       </c>
-      <c r="D4" s="31">
+      <c r="D4" s="30">
         <f>'Data from BFPIaE'!D6/'Data from BFPIaE'!B6</f>
-        <v>0.15500746052469119</v>
+        <v>1.29291393709361</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
@@ -1890,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>35</v>
       </c>
@@ -1903,7 +1926,7 @@
       <c r="D5" s="8">
         <v>0</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="30">
         <f>'Data from BFPIaE'!D7/'Data from BFPIaE'!B7</f>
         <v>0</v>
       </c>
@@ -1959,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A6" s="7" t="s">
         <v>36</v>
       </c>
@@ -2027,7 +2050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
@@ -2095,7 +2118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A8" s="7" t="s">
         <v>38</v>
       </c>
@@ -2163,7 +2186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
@@ -2188,9 +2211,9 @@
       <c r="H9" s="11">
         <v>0</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="30">
         <f>'Data from BFPIaE'!D11/'Data from BFPIaE'!B11</f>
-        <v>0.68036965837987495</v>
+        <v>4.3499342732737992E-2</v>
       </c>
       <c r="J9" s="8">
         <v>0</v>
@@ -2232,7 +2255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A10" s="6" t="s">
         <v>40</v>
       </c>
@@ -2262,7 +2285,7 @@
       </c>
       <c r="J10" s="12">
         <f>'Data from BFPIaE'!D12/SUM('Data from BFPIaE'!D12:E12)</f>
-        <v>7.2806513229885905E-2</v>
+        <v>0.57310527529393351</v>
       </c>
       <c r="K10" s="8">
         <v>0</v>
@@ -2287,7 +2310,7 @@
       </c>
       <c r="R10" s="13">
         <f>1-J10</f>
-        <v>0.92719348677011415</v>
+        <v>0.42689472470606649</v>
       </c>
       <c r="S10" s="8">
         <v>0</v>
@@ -2302,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>41</v>
       </c>
@@ -2335,7 +2358,7 @@
       </c>
       <c r="K11" s="12">
         <f>'Data from BFPIaE'!D13/SUM('Data from BFPIaE'!D13:E13)</f>
-        <v>0.26002912808189416</v>
+        <v>0.30464764504874542</v>
       </c>
       <c r="L11" s="8">
         <v>0</v>
@@ -2357,7 +2380,7 @@
       </c>
       <c r="R11" s="13">
         <f>1-K11</f>
-        <v>0.73997087191810584</v>
+        <v>0.69535235495125458</v>
       </c>
       <c r="S11" s="8">
         <v>0</v>
@@ -2372,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>42</v>
       </c>
@@ -2406,9 +2429,9 @@
       <c r="K12" s="8">
         <v>0</v>
       </c>
-      <c r="L12" s="31">
+      <c r="L12" s="30">
         <f>'Data from BFPIaE'!D14/'Data from BFPIaE'!B14</f>
-        <v>0.10491259896601664</v>
+        <v>0.46689888888030506</v>
       </c>
       <c r="M12" s="8">
         <v>0</v>
@@ -2441,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>43</v>
       </c>
@@ -2478,9 +2501,9 @@
       <c r="L13" s="8">
         <v>0</v>
       </c>
-      <c r="M13" s="31">
+      <c r="M13" s="30">
         <f>'Data from BFPIaE'!D15/'Data from BFPIaE'!B15</f>
-        <v>7.0542950086431883E-2</v>
+        <v>0.53332117396078926</v>
       </c>
       <c r="N13" s="8">
         <v>0</v>
@@ -2510,7 +2533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>44</v>
       </c>
@@ -2552,7 +2575,7 @@
       </c>
       <c r="N14" s="12">
         <f>'Data from BFPIaE'!D16/SUM('Data from BFPIaE'!D16:E16)</f>
-        <v>9.9755024140854479E-2</v>
+        <v>0.2758231788504043</v>
       </c>
       <c r="O14" s="11">
         <v>0</v>
@@ -2565,7 +2588,7 @@
       </c>
       <c r="R14" s="13">
         <f>1-N14</f>
-        <v>0.90024497585914554</v>
+        <v>0.7241768211495957</v>
       </c>
       <c r="S14" s="8">
         <v>0</v>
@@ -2580,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A15" s="7" t="s">
         <v>45</v>
       </c>
@@ -2648,7 +2671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>46</v>
       </c>
@@ -2716,7 +2739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
@@ -2765,9 +2788,9 @@
       <c r="P17" s="11">
         <v>0</v>
       </c>
-      <c r="Q17" s="31">
+      <c r="Q17" s="30">
         <f>'Data from BFPIaE'!D19/'Data from BFPIaE'!B19</f>
-        <v>0</v>
+        <v>1.6349895170843336E-2</v>
       </c>
       <c r="R17" s="8">
         <v>0</v>
@@ -2785,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>48</v>
       </c>
@@ -2853,7 +2876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>49</v>
       </c>
@@ -2907,11 +2930,11 @@
       </c>
       <c r="R19" s="13">
         <f>1-S19</f>
-        <v>0.49404181432894001</v>
+        <v>0.50069811636560213</v>
       </c>
       <c r="S19" s="12">
         <f>'Data from BFPIaE'!D21/SUM('Data from BFPIaE'!D21:E21)</f>
-        <v>0.50595818567105999</v>
+        <v>0.49930188363439781</v>
       </c>
       <c r="T19" s="8">
         <v>0</v>
@@ -2923,7 +2946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>50</v>
       </c>
@@ -2977,14 +3000,14 @@
       </c>
       <c r="R20" s="13">
         <f>1-T20</f>
-        <v>0.57774176716224113</v>
+        <v>0.76928917424872134</v>
       </c>
       <c r="S20" s="8">
         <v>0</v>
       </c>
       <c r="T20" s="12">
         <f>'Data from BFPIaE'!D22/SUM('Data from BFPIaE'!D22:E22)</f>
-        <v>0.42225823283775882</v>
+        <v>0.23071082575127866</v>
       </c>
       <c r="U20" s="8">
         <v>0</v>
@@ -2993,7 +3016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A21" s="6" t="s">
         <v>51</v>
       </c>
@@ -3054,15 +3077,15 @@
       <c r="T21" s="8">
         <v>0</v>
       </c>
-      <c r="U21" s="31">
+      <c r="U21" s="30">
         <f>'Data from BFPIaE'!D23/'Data from BFPIaE'!B23</f>
-        <v>0</v>
+        <v>3.509506046633555E-3</v>
       </c>
       <c r="V21" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>52</v>
       </c>
@@ -3126,7 +3149,7 @@
       <c r="U22" s="8">
         <v>0</v>
       </c>
-      <c r="V22" s="31">
+      <c r="V22" s="30">
         <f>'Data from BFPIaE'!D24/'Data from BFPIaE'!B24</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Reverted fuels/BFPIaE to EU28 to align with other Agora updates and updated start year data in fuels/PoFDCtAE
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80BA74C-9054-4E84-AED9-CE504ED44E4E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12591F01-C67B-4490-81DB-0F6B4E393AEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="-16935" windowWidth="15585" windowHeight="13515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7170" yWindow="-14955" windowWidth="15585" windowHeight="12495" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="103">
   <si>
     <t>PoFDCtAE Percentage of Fuel Demand Change that Alters Exports</t>
   </si>
@@ -244,9 +244,6 @@
     <t>Percentage Change in Demand that Alters Exports (dimensionless) - From type (below)  / To type (right)</t>
   </si>
   <si>
-    <t>Converted to BTU</t>
-  </si>
-  <si>
     <t>Fuel</t>
   </si>
   <si>
@@ -271,9 +268,6 @@
     <t>uranium</t>
   </si>
   <si>
-    <t>Start Year Data</t>
-  </si>
-  <si>
     <t>Overall Approach and Assumptions</t>
   </si>
   <si>
@@ -338,6 +332,18 @@
   </si>
   <si>
     <t>The EU version of this variable currently follows US assumptions and calculation methodology.</t>
+  </si>
+  <si>
+    <t>Share of Total Outflows</t>
+  </si>
+  <si>
+    <t>Secondary petroleum products highlighted in green</t>
+  </si>
+  <si>
+    <t>To align with plcy-schd/IT, the start year is 2018</t>
+  </si>
+  <si>
+    <t>Start Year Data from BFPIaE</t>
   </si>
 </sst>
 </file>
@@ -347,7 +353,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -373,6 +379,13 @@
     </font>
     <font>
       <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -424,7 +437,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -432,12 +445,93 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -472,56 +566,101 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -801,9 +940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -819,8 +956,8 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="25" t="s">
-        <v>79</v>
+      <c r="B3" s="16" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -859,13 +996,13 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B12" s="25" t="s">
-        <v>80</v>
+      <c r="B12" s="16" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B13" s="26" t="s">
-        <v>81</v>
+      <c r="B13" s="17" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
@@ -874,8 +1011,8 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="37" t="s">
-        <v>100</v>
+      <c r="A17" s="23" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
@@ -953,12 +1090,12 @@
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.45">
@@ -1007,44 +1144,44 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A49" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="B49" s="32"/>
+      <c r="A49" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B49" s="21"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.45">
@@ -1052,12 +1189,12 @@
         <v>53</v>
       </c>
       <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="15"/>
-      <c r="F59" s="15"/>
-      <c r="G59" s="15"/>
-      <c r="H59" s="15"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="37"/>
+      <c r="E59" s="37"/>
+      <c r="F59" s="37"/>
+      <c r="G59" s="37"/>
+      <c r="H59" s="37"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
@@ -1106,7 +1243,7 @@
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.45">
@@ -1148,473 +1285,657 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="B1:L29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="44.1328125" customWidth="1"/>
-    <col min="2" max="5" width="15.3984375" customWidth="1"/>
-    <col min="6" max="6" width="12.86328125" customWidth="1"/>
-    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="100.73046875" customWidth="1"/>
+    <col min="1" max="1" width="0.3984375" customWidth="1"/>
+    <col min="2" max="2" width="44.1328125" customWidth="1"/>
+    <col min="3" max="6" width="15.3984375" customWidth="1"/>
+    <col min="7" max="7" width="12.86328125" customWidth="1"/>
+    <col min="8" max="8" width="1.9296875" customWidth="1"/>
+    <col min="9" max="9" width="10.59765625" customWidth="1"/>
+    <col min="10" max="10" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="1.9296875" customWidth="1"/>
+    <col min="12" max="12" width="100.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" s="14" t="s">
+    <row r="1" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B2" s="56" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B3" s="59" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="61"/>
+      <c r="I3" s="38" t="s">
+        <v>99</v>
+      </c>
+      <c r="J3" s="39"/>
+      <c r="L3" s="18" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B4" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="17"/>
-      <c r="H2" s="28" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="18" t="s">
+      <c r="C4" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="D4" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="E4" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="F4" s="64" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="G4" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="I4" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B5" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="28"/>
+      <c r="I5" s="27"/>
+      <c r="J5" s="28"/>
+      <c r="L5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B6" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="43">
+        <v>1700249764545967.5</v>
+      </c>
+      <c r="D6" s="43">
+        <v>4402449843262403</v>
+      </c>
+      <c r="E6" s="43">
+        <v>479842820399329.38</v>
+      </c>
+      <c r="F6" s="44">
+        <f>C6+D6-E6</f>
+        <v>5622856787409041</v>
+      </c>
+      <c r="G6" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H6" s="24"/>
+      <c r="I6" s="29">
+        <f>E6/SUM($E6:$F6)</f>
+        <v>7.8627959958142646E-2</v>
+      </c>
+      <c r="J6" s="30">
+        <f>F6/SUM($E6:$F6)</f>
+        <v>0.92137204004185747</v>
+      </c>
+      <c r="K6" s="24"/>
+      <c r="L6" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="23"/>
-      <c r="H4" t="s">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B7" s="42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="43">
+        <v>3731101238123569</v>
+      </c>
+      <c r="D7" s="43">
+        <v>1.4659292018135964E+16</v>
+      </c>
+      <c r="E7" s="43">
+        <v>2610080945157157.5</v>
+      </c>
+      <c r="F7" s="44">
+        <f t="shared" ref="F7:F25" si="0">C7+D7-E7</f>
+        <v>1.5780312311102374E+16</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7" s="24"/>
+      <c r="I7" s="29">
+        <f t="shared" ref="I7:J8" si="1">E7/SUM($E7:$F7)</f>
+        <v>0.14192632581517881</v>
+      </c>
+      <c r="J7" s="30">
+        <f t="shared" si="1"/>
+        <v>0.85807367418482117</v>
+      </c>
+      <c r="K7" s="24"/>
+      <c r="L7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="33">
-        <v>1769370385808722.5</v>
-      </c>
-      <c r="C5" s="33">
-        <v>4304727594014679</v>
-      </c>
-      <c r="D5" s="33">
-        <v>530234220881090.13</v>
-      </c>
-      <c r="E5" s="34">
-        <f>B5+C5-D5</f>
-        <v>5543863758942312</v>
-      </c>
-      <c r="F5" t="s">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B8" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" t="s">
+      <c r="C8" s="43">
+        <v>8325482325117894</v>
+      </c>
+      <c r="D8" s="43">
+        <v>7896311820186260</v>
+      </c>
+      <c r="E8" s="43">
+        <v>0</v>
+      </c>
+      <c r="F8" s="44">
+        <f t="shared" si="0"/>
+        <v>1.6221794145304154E+16</v>
+      </c>
+      <c r="G8" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="24"/>
+      <c r="I8" s="29">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K8" s="24"/>
+      <c r="L8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="33">
-        <v>2663650455112149.5</v>
-      </c>
-      <c r="C6" s="33">
-        <v>1.396792574668349E+16</v>
-      </c>
-      <c r="D6" s="33">
-        <v>3443870796960235.5</v>
-      </c>
-      <c r="E6" s="34">
-        <f t="shared" ref="E6:E24" si="0">B6+C6-D6</f>
-        <v>1.3187705404835404E+16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="29"/>
-      <c r="H6" t="s">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B9" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="27"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="24"/>
+      <c r="L9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" s="33">
-        <v>7762103858922054</v>
-      </c>
-      <c r="C7" s="33">
-        <v>8804296582606409</v>
-      </c>
-      <c r="D7" s="33">
-        <v>0</v>
-      </c>
-      <c r="E7" s="34">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B10" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="24"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B11" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="24"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B12" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="43">
+        <v>4427401291031379</v>
+      </c>
+      <c r="D12" s="43">
+        <v>447002167542935.63</v>
+      </c>
+      <c r="E12" s="43">
+        <v>197730276062586.31</v>
+      </c>
+      <c r="F12" s="44">
         <f t="shared" si="0"/>
-        <v>1.6566400441528464E+16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G7" s="29"/>
-      <c r="H7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A8" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="29"/>
-      <c r="H8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="29"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="29"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="33">
-        <v>4165397947498852.5</v>
-      </c>
-      <c r="C11" s="33">
-        <v>312642855049688.31</v>
-      </c>
-      <c r="D11" s="33">
-        <v>181192072936495.97</v>
-      </c>
-      <c r="E11" s="34">
+        <v>4676673182511729</v>
+      </c>
+      <c r="G12" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="24"/>
+      <c r="I12" s="29">
+        <f t="shared" ref="I12:J17" si="2">E12/SUM($E12:$F12)</f>
+        <v>4.0565020467226418E-2</v>
+      </c>
+      <c r="J12" s="30">
+        <f t="shared" si="2"/>
+        <v>0.95943497953277368</v>
+      </c>
+      <c r="K12" s="24"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B13" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="49">
+        <v>4920569229684010</v>
+      </c>
+      <c r="D13" s="43">
+        <v>1027832055816836.6</v>
+      </c>
+      <c r="E13" s="43">
+        <v>3416763288927387</v>
+      </c>
+      <c r="F13" s="44">
         <f t="shared" si="0"/>
-        <v>4296848729612045</v>
-      </c>
-      <c r="F11" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="29"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A12" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="35">
-        <v>4199805007475681</v>
-      </c>
-      <c r="C12" s="33">
-        <v>1013941160881174.4</v>
-      </c>
-      <c r="D12" s="33">
-        <v>2988025433128846.5</v>
-      </c>
-      <c r="E12" s="34">
+        <v>2531637996573460</v>
+      </c>
+      <c r="G13" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="24"/>
+      <c r="I13" s="33">
+        <f t="shared" si="2"/>
+        <v>0.57440026738876959</v>
+      </c>
+      <c r="J13" s="34">
+        <f t="shared" si="2"/>
+        <v>0.42559973261123046</v>
+      </c>
+      <c r="K13" s="24"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B14" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="49">
+        <v>1.0016448997232614E+16</v>
+      </c>
+      <c r="D14" s="43">
+        <v>5201333461515337</v>
+      </c>
+      <c r="E14" s="43">
+        <v>4014349226614311</v>
+      </c>
+      <c r="F14" s="44">
         <f t="shared" si="0"/>
-        <v>2225720735228008.5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="29"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A13" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="35">
-        <v>9413120341769230</v>
-      </c>
-      <c r="C13" s="33">
-        <v>4830704037462619</v>
-      </c>
-      <c r="D13" s="33">
-        <v>4339347553620890.5</v>
-      </c>
-      <c r="E13" s="34">
+        <v>1.120343323213364E+16</v>
+      </c>
+      <c r="G14" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H14" s="24"/>
+      <c r="I14" s="33">
+        <f t="shared" si="2"/>
+        <v>0.26379331137741818</v>
+      </c>
+      <c r="J14" s="34">
+        <f t="shared" si="2"/>
+        <v>0.73620668862258176</v>
+      </c>
+      <c r="K14" s="24"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B15" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="43">
+        <v>104271668392538.86</v>
+      </c>
+      <c r="D15" s="43">
+        <v>63748993793056.195</v>
+      </c>
+      <c r="E15" s="43">
+        <v>48849723805629.555</v>
+      </c>
+      <c r="F15" s="44">
         <f t="shared" si="0"/>
-        <v>9904476825610958</v>
-      </c>
-      <c r="F13" t="s">
-        <v>76</v>
-      </c>
-      <c r="G13" s="29"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="33">
-        <v>89807897624285.297</v>
-      </c>
-      <c r="C14" s="33">
-        <v>50292782953843.539</v>
-      </c>
-      <c r="D14" s="33">
-        <v>41931207613454.992</v>
-      </c>
-      <c r="E14" s="34">
+        <v>119170938379965.5</v>
+      </c>
+      <c r="G15" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="24"/>
+      <c r="I15" s="29">
+        <f t="shared" si="2"/>
+        <v>0.29073640807146867</v>
+      </c>
+      <c r="J15" s="30">
+        <f t="shared" si="2"/>
+        <v>0.70926359192853128</v>
+      </c>
+      <c r="K15" s="24"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B16" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="43">
+        <v>509713332867213.69</v>
+      </c>
+      <c r="D16" s="43">
+        <v>346554845501331.81</v>
+      </c>
+      <c r="E16" s="43">
+        <v>293750693131906.88</v>
+      </c>
+      <c r="F16" s="44">
         <f t="shared" si="0"/>
-        <v>98169472964673.844</v>
-      </c>
-      <c r="F14" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="29"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="33">
-        <v>470056326182592.56</v>
-      </c>
-      <c r="C15" s="33">
-        <v>252654197726164</v>
-      </c>
-      <c r="D15" s="33">
-        <v>250690991707395.94</v>
-      </c>
-      <c r="E15" s="34">
+        <v>562517485236638.63</v>
+      </c>
+      <c r="G16" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H16" s="24"/>
+      <c r="I16" s="29">
+        <f t="shared" si="2"/>
+        <v>0.34305921970800363</v>
+      </c>
+      <c r="J16" s="30">
+        <f t="shared" si="2"/>
+        <v>0.65694078029199643</v>
+      </c>
+      <c r="K16" s="24"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B17" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="49">
+        <v>1581179978156898.8</v>
+      </c>
+      <c r="D17" s="43">
+        <v>1508087219315272.8</v>
+      </c>
+      <c r="E17" s="43">
+        <v>773650324741610.75</v>
+      </c>
+      <c r="F17" s="44">
         <f t="shared" si="0"/>
-        <v>472019532201360.56</v>
-      </c>
-      <c r="F15" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" s="29"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A16" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="35">
-        <v>1242913561157512.5</v>
-      </c>
-      <c r="C16" s="33">
-        <v>1046968038949733</v>
-      </c>
-      <c r="D16" s="33">
-        <v>631602422132630.75</v>
-      </c>
-      <c r="E16" s="34">
+        <v>2315616872730561</v>
+      </c>
+      <c r="G17" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H17" s="24"/>
+      <c r="I17" s="33">
+        <f t="shared" si="2"/>
+        <v>0.25043166397994288</v>
+      </c>
+      <c r="J17" s="34">
+        <f t="shared" si="2"/>
+        <v>0.74956833602005701</v>
+      </c>
+      <c r="K17" s="24"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B18" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="24"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B19" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="24"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B20" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="43">
+        <v>3082731931132596</v>
+      </c>
+      <c r="D20" s="43">
+        <v>37546912707632.57</v>
+      </c>
+      <c r="E20" s="43">
+        <v>50559840853480.148</v>
+      </c>
+      <c r="F20" s="44">
         <f t="shared" si="0"/>
-        <v>1658279177974614.8</v>
-      </c>
-      <c r="F16" t="s">
-        <v>76</v>
-      </c>
-      <c r="G16" s="29"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A17" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="29"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A18" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="29"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A19" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="33">
-        <v>3160571929646474.5</v>
-      </c>
-      <c r="C19" s="33">
-        <v>38203004039936.016</v>
-      </c>
-      <c r="D19" s="33">
-        <v>51675019729629.898</v>
-      </c>
-      <c r="E19" s="34">
+        <v>3069719002986748.5</v>
+      </c>
+      <c r="G20" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H20" s="24"/>
+      <c r="I20" s="29">
+        <f t="shared" ref="I20:J25" si="3">E20/SUM($E20:$F20)</f>
+        <v>1.6203629029274354E-2</v>
+      </c>
+      <c r="J20" s="30">
+        <f t="shared" si="3"/>
+        <v>0.9837963709707257</v>
+      </c>
+      <c r="K20" s="24"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B21" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="43">
+        <v>2803472740950065.5</v>
+      </c>
+      <c r="D21" s="43">
+        <v>2.2396832094073788E+16</v>
+      </c>
+      <c r="E21" s="43">
+        <v>1856053932251206</v>
+      </c>
+      <c r="F21" s="44">
         <f t="shared" si="0"/>
-        <v>3147099913956780.5</v>
-      </c>
-      <c r="F19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G19" s="29"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A20" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="33">
-        <v>875407792588829.88</v>
-      </c>
-      <c r="C20" s="33">
-        <v>2.0931542682938876E+16</v>
-      </c>
-      <c r="D20" s="33">
-        <v>242821039629142.72</v>
-      </c>
-      <c r="E20" s="34">
+        <v>2.3344250902772648E+16</v>
+      </c>
+      <c r="G21" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H21" s="24"/>
+      <c r="I21" s="29">
+        <f t="shared" si="3"/>
+        <v>7.3652042878133261E-2</v>
+      </c>
+      <c r="J21" s="30">
+        <f t="shared" si="3"/>
+        <v>0.92634795712186668</v>
+      </c>
+      <c r="K21" s="24"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B22" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="49">
+        <v>2864838130127541.5</v>
+      </c>
+      <c r="D22" s="43">
+        <v>1739549700086853</v>
+      </c>
+      <c r="E22" s="43">
+        <v>2207934520447625</v>
+      </c>
+      <c r="F22" s="44">
         <f t="shared" si="0"/>
-        <v>2.156412943589856E+16</v>
-      </c>
-      <c r="F20" t="s">
-        <v>76</v>
-      </c>
-      <c r="G20" s="29"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A21" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="35">
-        <v>2796362077584358.5</v>
-      </c>
-      <c r="C21" s="33">
-        <v>1705325640848346.3</v>
-      </c>
-      <c r="D21" s="33">
-        <v>2247701157347284.3</v>
-      </c>
-      <c r="E21" s="34">
+        <v>2396453309766769</v>
+      </c>
+      <c r="G22" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H22" s="24"/>
+      <c r="I22" s="33">
+        <f t="shared" si="3"/>
+        <v>0.47952835466182198</v>
+      </c>
+      <c r="J22" s="34">
+        <f t="shared" si="3"/>
+        <v>0.52047164533817802</v>
+      </c>
+      <c r="K22" s="24"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B23" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="49">
+        <v>699625641777144.63</v>
+      </c>
+      <c r="D23" s="43">
+        <v>973690848165933.5</v>
+      </c>
+      <c r="E23" s="43">
+        <v>372113118016514.13</v>
+      </c>
+      <c r="F23" s="44">
         <f t="shared" si="0"/>
-        <v>2253986561085421</v>
-      </c>
-      <c r="F21" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="29"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A22" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="35">
-        <v>629613892336042.38</v>
-      </c>
-      <c r="C22" s="33">
-        <v>868822141238955.25</v>
-      </c>
-      <c r="D22" s="33">
-        <v>345705414641558.38</v>
-      </c>
-      <c r="E22" s="34">
+        <v>1301203371926564</v>
+      </c>
+      <c r="G23" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23" s="24"/>
+      <c r="I23" s="33">
+        <f t="shared" si="3"/>
+        <v>0.22238059581255454</v>
+      </c>
+      <c r="J23" s="34">
+        <f t="shared" si="3"/>
+        <v>0.77761940418744557</v>
+      </c>
+      <c r="K23" s="24"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B24" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="50">
+        <v>975362274371115.75</v>
+      </c>
+      <c r="D24" s="43">
+        <v>37256319561081.477</v>
+      </c>
+      <c r="E24" s="43">
+        <v>3055762395890.1348</v>
+      </c>
+      <c r="F24" s="44">
         <f t="shared" si="0"/>
-        <v>1152730618933439</v>
-      </c>
-      <c r="F22" t="s">
-        <v>76</v>
-      </c>
-      <c r="G22" s="29"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A23" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="36">
-        <v>878812251216380.5</v>
-      </c>
-      <c r="C23" s="33">
-        <v>37448814583497.266</v>
-      </c>
-      <c r="D23" s="33">
-        <v>3084196909499.5342</v>
-      </c>
-      <c r="E23" s="34">
+        <v>1009562831536307.1</v>
+      </c>
+      <c r="G24" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H24" s="24"/>
+      <c r="I24" s="29">
+        <f t="shared" si="3"/>
+        <v>3.0176834735218599E-3</v>
+      </c>
+      <c r="J24" s="30">
+        <f t="shared" si="3"/>
+        <v>0.99698231652647817</v>
+      </c>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B25" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="52">
+        <v>2421651727.5342541</v>
+      </c>
+      <c r="D25" s="53">
+        <v>0</v>
+      </c>
+      <c r="E25" s="53">
+        <v>0</v>
+      </c>
+      <c r="F25" s="54">
         <f t="shared" si="0"/>
-        <v>913176868890378.25</v>
-      </c>
-      <c r="F23" t="s">
-        <v>76</v>
-      </c>
-      <c r="G23" s="29"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A24" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" s="36">
-        <v>1290868995.2225955</v>
-      </c>
-      <c r="C24" s="33">
-        <v>0</v>
-      </c>
-      <c r="D24" s="33">
-        <v>0</v>
-      </c>
-      <c r="E24" s="34">
-        <f t="shared" si="0"/>
-        <v>1290868995.2225955</v>
-      </c>
-      <c r="F24" t="s">
-        <v>76</v>
-      </c>
-      <c r="G24" s="29"/>
+        <v>2421651727.5342541</v>
+      </c>
+      <c r="G25" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="H25" s="24"/>
+      <c r="I25" s="31">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="32">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K25" s="24"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B28" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="36"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="F29" s="22"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I3:J3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1626,11 +1947,11 @@
   </sheetPr>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1782,9 +2103,9 @@
       <c r="B3" s="11">
         <v>0</v>
       </c>
-      <c r="C3" s="30">
-        <f>'Data from BFPIaE'!D5/'Data from BFPIaE'!B5</f>
-        <v>0.29967395472075625</v>
+      <c r="C3" s="19">
+        <f>'Data from BFPIaE'!E6/'Data from BFPIaE'!C6</f>
+        <v>0.2822190188789504</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
@@ -1854,9 +2175,9 @@
       <c r="C4" s="8">
         <v>0</v>
       </c>
-      <c r="D4" s="30">
-        <f>'Data from BFPIaE'!D6/'Data from BFPIaE'!B6</f>
-        <v>1.29291393709361</v>
+      <c r="D4" s="19">
+        <f>'Data from BFPIaE'!E7/'Data from BFPIaE'!C7</f>
+        <v>0.69954707164949759</v>
       </c>
       <c r="E4" s="8">
         <v>0</v>
@@ -1926,8 +2247,8 @@
       <c r="D5" s="8">
         <v>0</v>
       </c>
-      <c r="E5" s="30">
-        <f>'Data from BFPIaE'!D7/'Data from BFPIaE'!B7</f>
+      <c r="E5" s="19">
+        <f>'Data from BFPIaE'!E8/'Data from BFPIaE'!C8</f>
         <v>0</v>
       </c>
       <c r="F5" s="11">
@@ -2211,9 +2532,9 @@
       <c r="H9" s="11">
         <v>0</v>
       </c>
-      <c r="I9" s="30">
-        <f>'Data from BFPIaE'!D11/'Data from BFPIaE'!B11</f>
-        <v>4.3499342732737992E-2</v>
+      <c r="I9" s="19">
+        <f>'Data from BFPIaE'!E12/'Data from BFPIaE'!C12</f>
+        <v>4.4660572436279959E-2</v>
       </c>
       <c r="J9" s="8">
         <v>0</v>
@@ -2284,8 +2605,8 @@
         <v>0</v>
       </c>
       <c r="J10" s="12">
-        <f>'Data from BFPIaE'!D12/SUM('Data from BFPIaE'!D12:E12)</f>
-        <v>0.57310527529393351</v>
+        <f>'Data from BFPIaE'!E13/SUM('Data from BFPIaE'!E13:F13)</f>
+        <v>0.57440026738876959</v>
       </c>
       <c r="K10" s="8">
         <v>0</v>
@@ -2310,7 +2631,7 @@
       </c>
       <c r="R10" s="13">
         <f>1-J10</f>
-        <v>0.42689472470606649</v>
+        <v>0.42559973261123041</v>
       </c>
       <c r="S10" s="8">
         <v>0</v>
@@ -2357,8 +2678,8 @@
         <v>0</v>
       </c>
       <c r="K11" s="12">
-        <f>'Data from BFPIaE'!D13/SUM('Data from BFPIaE'!D13:E13)</f>
-        <v>0.30464764504874542</v>
+        <f>'Data from BFPIaE'!E14/SUM('Data from BFPIaE'!E14:F14)</f>
+        <v>0.26379331137741818</v>
       </c>
       <c r="L11" s="8">
         <v>0</v>
@@ -2380,7 +2701,7 @@
       </c>
       <c r="R11" s="13">
         <f>1-K11</f>
-        <v>0.69535235495125458</v>
+        <v>0.73620668862258176</v>
       </c>
       <c r="S11" s="8">
         <v>0</v>
@@ -2429,9 +2750,9 @@
       <c r="K12" s="8">
         <v>0</v>
       </c>
-      <c r="L12" s="30">
-        <f>'Data from BFPIaE'!D14/'Data from BFPIaE'!B14</f>
-        <v>0.46689888888030506</v>
+      <c r="L12" s="19">
+        <f>'Data from BFPIaE'!E15/'Data from BFPIaE'!C15</f>
+        <v>0.46848510778336205</v>
       </c>
       <c r="M12" s="8">
         <v>0</v>
@@ -2501,9 +2822,9 @@
       <c r="L13" s="8">
         <v>0</v>
       </c>
-      <c r="M13" s="30">
-        <f>'Data from BFPIaE'!D15/'Data from BFPIaE'!B15</f>
-        <v>0.53332117396078926</v>
+      <c r="M13" s="19">
+        <f>'Data from BFPIaE'!E16/'Data from BFPIaE'!C16</f>
+        <v>0.57630568829642992</v>
       </c>
       <c r="N13" s="8">
         <v>0</v>
@@ -2574,8 +2895,8 @@
         <v>0</v>
       </c>
       <c r="N14" s="12">
-        <f>'Data from BFPIaE'!D16/SUM('Data from BFPIaE'!D16:E16)</f>
-        <v>0.2758231788504043</v>
+        <f>'Data from BFPIaE'!E17/SUM('Data from BFPIaE'!E17:F17)</f>
+        <v>0.25043166397994288</v>
       </c>
       <c r="O14" s="11">
         <v>0</v>
@@ -2588,7 +2909,7 @@
       </c>
       <c r="R14" s="13">
         <f>1-N14</f>
-        <v>0.7241768211495957</v>
+        <v>0.74956833602005712</v>
       </c>
       <c r="S14" s="8">
         <v>0</v>
@@ -2788,9 +3109,9 @@
       <c r="P17" s="11">
         <v>0</v>
       </c>
-      <c r="Q17" s="30">
-        <f>'Data from BFPIaE'!D19/'Data from BFPIaE'!B19</f>
-        <v>1.6349895170843336E-2</v>
+      <c r="Q17" s="19">
+        <f>'Data from BFPIaE'!E20/'Data from BFPIaE'!C20</f>
+        <v>1.6400985224461102E-2</v>
       </c>
       <c r="R17" s="8">
         <v>0</v>
@@ -2930,11 +3251,11 @@
       </c>
       <c r="R19" s="13">
         <f>1-S19</f>
-        <v>0.50069811636560213</v>
+        <v>0.52047164533817802</v>
       </c>
       <c r="S19" s="12">
-        <f>'Data from BFPIaE'!D21/SUM('Data from BFPIaE'!D21:E21)</f>
-        <v>0.49930188363439781</v>
+        <f>'Data from BFPIaE'!E22/SUM('Data from BFPIaE'!E22:F22)</f>
+        <v>0.47952835466182198</v>
       </c>
       <c r="T19" s="8">
         <v>0</v>
@@ -3000,14 +3321,14 @@
       </c>
       <c r="R20" s="13">
         <f>1-T20</f>
-        <v>0.76928917424872134</v>
+        <v>0.77761940418744546</v>
       </c>
       <c r="S20" s="8">
         <v>0</v>
       </c>
       <c r="T20" s="12">
-        <f>'Data from BFPIaE'!D22/SUM('Data from BFPIaE'!D22:E22)</f>
-        <v>0.23071082575127866</v>
+        <f>'Data from BFPIaE'!E23/SUM('Data from BFPIaE'!E23:F23)</f>
+        <v>0.22238059581255454</v>
       </c>
       <c r="U20" s="8">
         <v>0</v>
@@ -3077,9 +3398,9 @@
       <c r="T21" s="8">
         <v>0</v>
       </c>
-      <c r="U21" s="30">
-        <f>'Data from BFPIaE'!D23/'Data from BFPIaE'!B23</f>
-        <v>3.509506046633555E-3</v>
+      <c r="U21" s="19">
+        <f>'Data from BFPIaE'!E24/'Data from BFPIaE'!C24</f>
+        <v>3.1329511876603986E-3</v>
       </c>
       <c r="V21" s="8">
         <v>0</v>
@@ -3149,8 +3470,8 @@
       <c r="U22" s="8">
         <v>0</v>
       </c>
-      <c r="V22" s="30">
-        <f>'Data from BFPIaE'!D24/'Data from BFPIaE'!B24</f>
+      <c r="V22" s="19">
+        <f>'Data from BFPIaE'!E25/'Data from BFPIaE'!C25</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update About tab for fuels/PoFDCtAE
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\fuels\PoFDCtAE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12591F01-C67B-4490-81DB-0F6B4E393AEC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7170" yWindow="-14955" windowWidth="15585" windowHeight="12495" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7170" yWindow="-14955" windowWidth="15585" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data from BFPIaE" sheetId="3" r:id="rId2"/>
     <sheet name="PoFDCtAE" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="104">
   <si>
     <t>PoFDCtAE Percentage of Fuel Demand Change that Alters Exports</t>
   </si>
@@ -304,9 +303,6 @@
     <t>Example 1: Saudi Arabia</t>
   </si>
   <si>
-    <t>United States Settings</t>
-  </si>
-  <si>
     <t>Based on consultation with oil market experts at Rapidian Energy and Wood Mackenzie,</t>
   </si>
   <si>
@@ -344,12 +340,18 @@
   </si>
   <si>
     <t>Start Year Data from BFPIaE</t>
+  </si>
+  <si>
+    <t>United States and EU Settings</t>
+  </si>
+  <si>
+    <t>We choose to use the same assumptions for the EU.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
@@ -598,12 +600,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -655,6 +651,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -937,10 +939,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H76"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H78"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD60"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1012,7 +1016,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
@@ -1145,138 +1149,143 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49" s="20" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="B49" s="21"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A59" s="14" t="s">
+      <c r="A59" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A61" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="B59" s="15"/>
-      <c r="C59" s="37"/>
-      <c r="D59" s="37"/>
-      <c r="E59" s="37"/>
-      <c r="F59" s="37"/>
-      <c r="G59" s="37"/>
-      <c r="H59" s="37"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>55</v>
-      </c>
+      <c r="B61" s="15"/>
+      <c r="C61" s="37"/>
+      <c r="D61" s="37"/>
+      <c r="E61" s="37"/>
+      <c r="F61" s="37"/>
+      <c r="G61" s="37"/>
+      <c r="H61" s="37"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>59</v>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A66" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>97</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>66</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
         <v>62</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="B10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId1"/>
+    <hyperlink ref="B8" r:id="rId2"/>
+    <hyperlink ref="B9" r:id="rId3"/>
+    <hyperlink ref="B10" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -1284,7 +1293,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:L29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1306,49 +1315,49 @@
   <sheetData>
     <row r="1" spans="2:12" ht="3" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B2" s="56" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
+      <c r="B2" s="54" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="56"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B3" s="59" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
-      <c r="I3" s="38" t="s">
-        <v>99</v>
-      </c>
-      <c r="J3" s="39"/>
+      <c r="B3" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="59"/>
+      <c r="I3" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="J3" s="65"/>
       <c r="L3" s="18" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B4" s="62" t="s">
+      <c r="B4" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="63" t="s">
+      <c r="E4" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="64" t="s">
+      <c r="F4" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="65" t="s">
+      <c r="G4" s="63" t="s">
         <v>74</v>
       </c>
       <c r="I4" s="25" t="s">
@@ -1362,13 +1371,13 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
       <c r="G5" s="28"/>
       <c r="I5" s="27"/>
       <c r="J5" s="28"/>
@@ -1377,23 +1386,23 @@
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="43">
+      <c r="C6" s="41">
         <v>1700249764545967.5</v>
       </c>
-      <c r="D6" s="43">
+      <c r="D6" s="41">
         <v>4402449843262403</v>
       </c>
-      <c r="E6" s="43">
+      <c r="E6" s="41">
         <v>479842820399329.38</v>
       </c>
-      <c r="F6" s="44">
+      <c r="F6" s="42">
         <f>C6+D6-E6</f>
         <v>5622856787409041</v>
       </c>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H6" s="24"/>
@@ -1411,23 +1420,23 @@
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="43">
+      <c r="C7" s="41">
         <v>3731101238123569</v>
       </c>
-      <c r="D7" s="43">
+      <c r="D7" s="41">
         <v>1.4659292018135964E+16</v>
       </c>
-      <c r="E7" s="43">
+      <c r="E7" s="41">
         <v>2610080945157157.5</v>
       </c>
-      <c r="F7" s="44">
+      <c r="F7" s="42">
         <f t="shared" ref="F7:F25" si="0">C7+D7-E7</f>
         <v>1.5780312311102374E+16</v>
       </c>
-      <c r="G7" s="45" t="s">
+      <c r="G7" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H7" s="24"/>
@@ -1445,23 +1454,23 @@
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="C8" s="43">
+      <c r="C8" s="41">
         <v>8325482325117894</v>
       </c>
-      <c r="D8" s="43">
+      <c r="D8" s="41">
         <v>7896311820186260</v>
       </c>
-      <c r="E8" s="43">
-        <v>0</v>
-      </c>
-      <c r="F8" s="44">
+      <c r="E8" s="41">
+        <v>0</v>
+      </c>
+      <c r="F8" s="42">
         <f t="shared" si="0"/>
         <v>1.6221794145304154E+16</v>
       </c>
-      <c r="G8" s="45" t="s">
+      <c r="G8" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H8" s="24"/>
@@ -1479,13 +1488,13 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="41"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="28"/>
       <c r="H9" s="24"/>
       <c r="I9" s="27"/>
@@ -1496,13 +1505,13 @@
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="41"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="28"/>
       <c r="H10" s="24"/>
       <c r="I10" s="27"/>
@@ -1510,13 +1519,13 @@
       <c r="K10" s="24"/>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="41"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="28"/>
       <c r="H11" s="24"/>
       <c r="I11" s="27"/>
@@ -1524,23 +1533,23 @@
       <c r="K11" s="24"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="43">
+      <c r="C12" s="41">
         <v>4427401291031379</v>
       </c>
-      <c r="D12" s="43">
+      <c r="D12" s="41">
         <v>447002167542935.63</v>
       </c>
-      <c r="E12" s="43">
+      <c r="E12" s="41">
         <v>197730276062586.31</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="42">
         <f t="shared" si="0"/>
         <v>4676673182511729</v>
       </c>
-      <c r="G12" s="45" t="s">
+      <c r="G12" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H12" s="24"/>
@@ -1555,23 +1564,23 @@
       <c r="K12" s="24"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="49">
+      <c r="C13" s="47">
         <v>4920569229684010</v>
       </c>
-      <c r="D13" s="43">
+      <c r="D13" s="41">
         <v>1027832055816836.6</v>
       </c>
-      <c r="E13" s="43">
+      <c r="E13" s="41">
         <v>3416763288927387</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="42">
         <f t="shared" si="0"/>
         <v>2531637996573460</v>
       </c>
-      <c r="G13" s="45" t="s">
+      <c r="G13" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H13" s="24"/>
@@ -1586,23 +1595,23 @@
       <c r="K13" s="24"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="49">
+      <c r="C14" s="47">
         <v>1.0016448997232614E+16</v>
       </c>
-      <c r="D14" s="43">
+      <c r="D14" s="41">
         <v>5201333461515337</v>
       </c>
-      <c r="E14" s="43">
+      <c r="E14" s="41">
         <v>4014349226614311</v>
       </c>
-      <c r="F14" s="44">
+      <c r="F14" s="42">
         <f t="shared" si="0"/>
         <v>1.120343323213364E+16</v>
       </c>
-      <c r="G14" s="45" t="s">
+      <c r="G14" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H14" s="24"/>
@@ -1617,23 +1626,23 @@
       <c r="K14" s="24"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="41">
         <v>104271668392538.86</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="41">
         <v>63748993793056.195</v>
       </c>
-      <c r="E15" s="43">
+      <c r="E15" s="41">
         <v>48849723805629.555</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="42">
         <f t="shared" si="0"/>
         <v>119170938379965.5</v>
       </c>
-      <c r="G15" s="45" t="s">
+      <c r="G15" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H15" s="24"/>
@@ -1648,23 +1657,23 @@
       <c r="K15" s="24"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="43">
+      <c r="C16" s="41">
         <v>509713332867213.69</v>
       </c>
-      <c r="D16" s="43">
+      <c r="D16" s="41">
         <v>346554845501331.81</v>
       </c>
-      <c r="E16" s="43">
+      <c r="E16" s="41">
         <v>293750693131906.88</v>
       </c>
-      <c r="F16" s="44">
+      <c r="F16" s="42">
         <f t="shared" si="0"/>
         <v>562517485236638.63</v>
       </c>
-      <c r="G16" s="45" t="s">
+      <c r="G16" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H16" s="24"/>
@@ -1679,23 +1688,23 @@
       <c r="K16" s="24"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="49">
+      <c r="C17" s="47">
         <v>1581179978156898.8</v>
       </c>
-      <c r="D17" s="43">
+      <c r="D17" s="41">
         <v>1508087219315272.8</v>
       </c>
-      <c r="E17" s="43">
+      <c r="E17" s="41">
         <v>773650324741610.75</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="42">
         <f t="shared" si="0"/>
         <v>2315616872730561</v>
       </c>
-      <c r="G17" s="45" t="s">
+      <c r="G17" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H17" s="24"/>
@@ -1710,13 +1719,13 @@
       <c r="K17" s="24"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="47"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="41"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="39"/>
       <c r="G18" s="28"/>
       <c r="H18" s="24"/>
       <c r="I18" s="27"/>
@@ -1724,13 +1733,13 @@
       <c r="K18" s="24"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="47"/>
-      <c r="D19" s="47"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="41"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
+      <c r="F19" s="39"/>
       <c r="G19" s="28"/>
       <c r="H19" s="24"/>
       <c r="I19" s="27"/>
@@ -1738,23 +1747,23 @@
       <c r="K19" s="24"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="43">
+      <c r="C20" s="41">
         <v>3082731931132596</v>
       </c>
-      <c r="D20" s="43">
+      <c r="D20" s="41">
         <v>37546912707632.57</v>
       </c>
-      <c r="E20" s="43">
+      <c r="E20" s="41">
         <v>50559840853480.148</v>
       </c>
-      <c r="F20" s="44">
+      <c r="F20" s="42">
         <f t="shared" si="0"/>
         <v>3069719002986748.5</v>
       </c>
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H20" s="24"/>
@@ -1769,23 +1778,23 @@
       <c r="K20" s="24"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="43">
+      <c r="C21" s="41">
         <v>2803472740950065.5</v>
       </c>
-      <c r="D21" s="43">
+      <c r="D21" s="41">
         <v>2.2396832094073788E+16</v>
       </c>
-      <c r="E21" s="43">
+      <c r="E21" s="41">
         <v>1856053932251206</v>
       </c>
-      <c r="F21" s="44">
+      <c r="F21" s="42">
         <f t="shared" si="0"/>
         <v>2.3344250902772648E+16</v>
       </c>
-      <c r="G21" s="45" t="s">
+      <c r="G21" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H21" s="24"/>
@@ -1800,23 +1809,23 @@
       <c r="K21" s="24"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B22" s="48" t="s">
+      <c r="B22" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="49">
+      <c r="C22" s="47">
         <v>2864838130127541.5</v>
       </c>
-      <c r="D22" s="43">
+      <c r="D22" s="41">
         <v>1739549700086853</v>
       </c>
-      <c r="E22" s="43">
+      <c r="E22" s="41">
         <v>2207934520447625</v>
       </c>
-      <c r="F22" s="44">
+      <c r="F22" s="42">
         <f t="shared" si="0"/>
         <v>2396453309766769</v>
       </c>
-      <c r="G22" s="45" t="s">
+      <c r="G22" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H22" s="24"/>
@@ -1831,23 +1840,23 @@
       <c r="K22" s="24"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B23" s="48" t="s">
+      <c r="B23" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="49">
+      <c r="C23" s="47">
         <v>699625641777144.63</v>
       </c>
-      <c r="D23" s="43">
+      <c r="D23" s="41">
         <v>973690848165933.5</v>
       </c>
-      <c r="E23" s="43">
+      <c r="E23" s="41">
         <v>372113118016514.13</v>
       </c>
-      <c r="F23" s="44">
+      <c r="F23" s="42">
         <f t="shared" si="0"/>
         <v>1301203371926564</v>
       </c>
-      <c r="G23" s="45" t="s">
+      <c r="G23" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H23" s="24"/>
@@ -1862,23 +1871,23 @@
       <c r="K23" s="24"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="50">
+      <c r="C24" s="48">
         <v>975362274371115.75</v>
       </c>
-      <c r="D24" s="43">
+      <c r="D24" s="41">
         <v>37256319561081.477</v>
       </c>
-      <c r="E24" s="43">
+      <c r="E24" s="41">
         <v>3055762395890.1348</v>
       </c>
-      <c r="F24" s="44">
+      <c r="F24" s="42">
         <f t="shared" si="0"/>
         <v>1009562831536307.1</v>
       </c>
-      <c r="G24" s="45" t="s">
+      <c r="G24" s="43" t="s">
         <v>75</v>
       </c>
       <c r="H24" s="24"/>
@@ -1893,23 +1902,23 @@
       <c r="K24" s="24"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.45">
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="52">
+      <c r="C25" s="50">
         <v>2421651727.5342541</v>
       </c>
-      <c r="D25" s="53">
-        <v>0</v>
-      </c>
-      <c r="E25" s="53">
-        <v>0</v>
-      </c>
-      <c r="F25" s="54">
+      <c r="D25" s="51">
+        <v>0</v>
+      </c>
+      <c r="E25" s="51">
+        <v>0</v>
+      </c>
+      <c r="F25" s="52">
         <f t="shared" si="0"/>
         <v>2421651727.5342541</v>
       </c>
-      <c r="G25" s="55" t="s">
+      <c r="G25" s="53" t="s">
         <v>75</v>
       </c>
       <c r="H25" s="24"/>
@@ -1925,7 +1934,7 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B28" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C28" s="36"/>
     </row>
@@ -1941,13 +1950,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:V22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>

</xml_diff>

<commit_message>
updating % fuel demand change for exports
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://energyinnovation.sharepoint.com/sites/EUEPSModeling/Shared Documents/InputData_Artelys/fuels/PoFDCtAE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{38FBEA54-9C77-4C4A-BC31-F0D1AFC59515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77318DDF-E0D6-433D-B9E1-17E6BF0D7043}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986ACDB5-CA33-45D5-8BAC-E4180D35192C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" firstSheet="2" activeTab="2" xr2:uid="{3E0B3505-0335-466F-B5FC-C5183A2DB44F}"/>
+    <workbookView xWindow="29970" yWindow="1170" windowWidth="30990" windowHeight="12645" activeTab="2" xr2:uid="{3E0B3505-0335-466F-B5FC-C5183A2DB44F}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -564,7 +564,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -643,44 +643,39 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -816,9 +811,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -856,7 +851,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -962,7 +957,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1104,7 +1099,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1114,32 +1109,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937B2E0C-144E-4608-927D-ACF1F00D1421}">
   <dimension ref="B10:D90"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="B34" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="10.90625" style="2"/>
-    <col min="3" max="3" width="44.26953125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.90625" style="2"/>
+    <col min="1" max="2" width="10.85546875" style="2"/>
+    <col min="3" max="3" width="44.28515625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
@@ -1150,7 +1145,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
         <v>87</v>
       </c>
@@ -1158,325 +1153,325 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C22" s="45" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C23" s="45" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C24" s="45"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C25" s="45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C26" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C27" s="45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C28" s="45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C29" s="45" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C30" s="45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C31" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C32" s="45" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C33" s="45"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C34" s="45" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C35" s="45"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C36" s="45" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C37" s="45"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C38" s="46" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C39" s="45" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C40" s="45" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C41" s="45" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C42" s="45" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C43" s="45" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C44" s="45" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C45" s="45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C46" s="45" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C47" s="45" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C48" s="45"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C49" s="47" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C50" s="45" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C51" s="45" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C52" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C53" s="45" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C54" s="45"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C55" s="45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C56" s="45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C57" s="45" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C58" s="45"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C59" s="45" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C60" s="45"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C61" s="47" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C62" s="45" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C63" s="45" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C64" s="45" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C65" s="45" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C66" s="45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C67" s="45" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C68" s="45"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C69" s="45" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C70" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C71" s="45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C72" s="45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C73" s="45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C74" s="45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C75" s="45"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C76" s="45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C77" s="45" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C78" s="45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="5"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="5"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="5"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B82" s="5"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="5"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="5"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B85" s="5"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="5"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="5"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B88" s="5"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="5"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="5"/>
     </row>
   </sheetData>
@@ -1493,27 +1488,27 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.54296875" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="57"/>
+      <c r="B1" s="57"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="50"/>
-      <c r="I1" s="50"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
         <v>52</v>
@@ -1523,14 +1518,14 @@
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="50"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="57"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
       <c r="B3" s="11" t="s">
         <v>89</v>
@@ -1541,17 +1536,17 @@
       <c r="F3" s="12"/>
       <c r="G3" s="13"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="J3" s="49"/>
+      <c r="J3" s="60"/>
       <c r="K3" s="7"/>
       <c r="L3" s="14" t="s">
         <v>54</v>
       </c>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="15" t="s">
         <v>55</v>
@@ -1584,7 +1579,7 @@
       </c>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="21" t="s">
         <v>61</v>
@@ -1603,7 +1598,7 @@
       </c>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="25" t="s">
         <v>63</v>
@@ -1639,7 +1634,7 @@
       </c>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
       <c r="B7" s="25" t="s">
         <v>65</v>
@@ -1675,7 +1670,7 @@
       </c>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7"/>
       <c r="B8" s="25" t="s">
         <v>67</v>
@@ -1711,7 +1706,7 @@
       </c>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="31" t="s">
         <v>68</v>
@@ -1730,7 +1725,7 @@
       </c>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="31" t="s">
         <v>70</v>
@@ -1743,11 +1738,11 @@
       <c r="H10" s="7"/>
       <c r="I10" s="40"/>
       <c r="J10" s="41"/>
-      <c r="K10" s="51"/>
-      <c r="L10" s="50"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="57"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="7"/>
       <c r="B11" s="31" t="s">
         <v>71</v>
@@ -1760,11 +1755,11 @@
       <c r="H11" s="7"/>
       <c r="I11" s="40"/>
       <c r="J11" s="41"/>
-      <c r="K11" s="51"/>
-      <c r="L11" s="50"/>
+      <c r="K11" s="58"/>
+      <c r="L11" s="57"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="25" t="s">
         <v>72</v>
@@ -1794,11 +1789,11 @@
         <f t="shared" si="1"/>
         <v>0.95507604016524161</v>
       </c>
-      <c r="K12" s="51"/>
-      <c r="L12" s="50"/>
+      <c r="K12" s="58"/>
+      <c r="L12" s="57"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="32" t="s">
         <v>73</v>
@@ -1828,11 +1823,11 @@
         <f t="shared" si="1"/>
         <v>0.3922833651703625</v>
       </c>
-      <c r="K13" s="51"/>
-      <c r="L13" s="50"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="57"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7"/>
       <c r="B14" s="32" t="s">
         <v>74</v>
@@ -1862,11 +1857,11 @@
         <f t="shared" si="1"/>
         <v>0.70550484210364817</v>
       </c>
-      <c r="K14" s="51"/>
-      <c r="L14" s="50"/>
+      <c r="K14" s="58"/>
+      <c r="L14" s="57"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7"/>
       <c r="B15" s="25" t="s">
         <v>75</v>
@@ -1896,11 +1891,11 @@
         <f t="shared" si="1"/>
         <v>0.71852702501386922</v>
       </c>
-      <c r="K15" s="51"/>
-      <c r="L15" s="50"/>
+      <c r="K15" s="58"/>
+      <c r="L15" s="57"/>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="25" t="s">
         <v>76</v>
@@ -1930,11 +1925,11 @@
         <f t="shared" si="1"/>
         <v>0.62841900526223626</v>
       </c>
-      <c r="K16" s="51"/>
-      <c r="L16" s="50"/>
+      <c r="K16" s="58"/>
+      <c r="L16" s="57"/>
       <c r="M16" s="7"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="32" t="s">
         <v>77</v>
@@ -1964,11 +1959,11 @@
         <f t="shared" si="1"/>
         <v>0.72086022686964368</v>
       </c>
-      <c r="K17" s="51"/>
-      <c r="L17" s="50"/>
+      <c r="K17" s="58"/>
+      <c r="L17" s="57"/>
       <c r="M17" s="7"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="31" t="s">
         <v>78</v>
@@ -1981,11 +1976,11 @@
       <c r="H18" s="7"/>
       <c r="I18" s="40"/>
       <c r="J18" s="41"/>
-      <c r="K18" s="51"/>
-      <c r="L18" s="50"/>
+      <c r="K18" s="58"/>
+      <c r="L18" s="57"/>
       <c r="M18" s="7"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="31" t="s">
         <v>79</v>
@@ -1998,11 +1993,11 @@
       <c r="H19" s="7"/>
       <c r="I19" s="40"/>
       <c r="J19" s="41"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="50"/>
+      <c r="K19" s="58"/>
+      <c r="L19" s="57"/>
       <c r="M19" s="7"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="25" t="s">
         <v>80</v>
@@ -2032,11 +2027,11 @@
         <f t="shared" si="1"/>
         <v>0.8807194770978013</v>
       </c>
-      <c r="K20" s="51"/>
-      <c r="L20" s="50"/>
+      <c r="K20" s="58"/>
+      <c r="L20" s="57"/>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="25" t="s">
         <v>81</v>
@@ -2066,11 +2061,11 @@
         <f t="shared" si="1"/>
         <v>0.99453702179044434</v>
       </c>
-      <c r="K21" s="51"/>
-      <c r="L21" s="50"/>
+      <c r="K21" s="58"/>
+      <c r="L21" s="57"/>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="32" t="s">
         <v>82</v>
@@ -2100,11 +2095,11 @@
         <f t="shared" si="1"/>
         <v>0.49856575142985632</v>
       </c>
-      <c r="K22" s="51"/>
-      <c r="L22" s="50"/>
+      <c r="K22" s="58"/>
+      <c r="L22" s="57"/>
       <c r="M22" s="7"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="32" t="s">
         <v>83</v>
@@ -2134,11 +2129,11 @@
         <f t="shared" si="1"/>
         <v>0.84498067686633227</v>
       </c>
-      <c r="K23" s="51"/>
-      <c r="L23" s="50"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="57"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="25" t="s">
         <v>84</v>
@@ -2168,11 +2163,11 @@
         <f t="shared" si="1"/>
         <v>0.9981760467937546</v>
       </c>
-      <c r="K24" s="51"/>
-      <c r="L24" s="50"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="57"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="34" t="s">
         <v>85</v>
@@ -2202,41 +2197,41 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K25" s="51"/>
-      <c r="L25" s="50"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="57"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="50"/>
-      <c r="B26" s="50"/>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="50"/>
-      <c r="I26" s="50"/>
+      <c r="H26" s="57"/>
+      <c r="I26" s="57"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="50"/>
-      <c r="L26" s="50"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="57"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="50"/>
-      <c r="B27" s="50"/>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="57"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="50"/>
-      <c r="I27" s="50"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="57"/>
       <c r="J27" s="7"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50"/>
+      <c r="K27" s="57"/>
+      <c r="L27" s="57"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="38" t="s">
         <v>86</v>
@@ -2246,63 +2241,51 @@
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="50"/>
-      <c r="I28" s="50"/>
+      <c r="H28" s="57"/>
+      <c r="I28" s="57"/>
       <c r="J28" s="7"/>
-      <c r="K28" s="50"/>
-      <c r="L28" s="50"/>
+      <c r="K28" s="57"/>
+      <c r="L28" s="57"/>
       <c r="M28" s="7"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="50"/>
-      <c r="B29" s="50"/>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="57"/>
+      <c r="B29" s="57"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
+      <c r="H29" s="57"/>
+      <c r="I29" s="57"/>
       <c r="J29" s="7"/>
-      <c r="K29" s="50"/>
-      <c r="L29" s="50"/>
+      <c r="K29" s="57"/>
+      <c r="L29" s="57"/>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="50"/>
-      <c r="B30" s="50"/>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="57"/>
+      <c r="B30" s="57"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="50"/>
-      <c r="I30" s="50"/>
+      <c r="H30" s="57"/>
+      <c r="I30" s="57"/>
       <c r="J30" s="7"/>
-      <c r="K30" s="50"/>
-      <c r="L30" s="50"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
       <c r="M30" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="K29:L29"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="K2:L2"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="K11:L11"/>
@@ -2315,12 +2298,24 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="K20:L20"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="K29:L29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2333,1571 +2328,1570 @@
   </sheetPr>
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="50" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="54" t="s">
+      <c r="D1" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="54" t="s">
+      <c r="E1" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="53" t="s">
+      <c r="H1" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="54" t="s">
+      <c r="K1" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="54" t="s">
+      <c r="L1" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="54" t="s">
+      <c r="N1" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="53" t="s">
+      <c r="O1" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="53" t="s">
+      <c r="P1" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="54" t="s">
+      <c r="Q1" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="54" t="s">
+      <c r="R1" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="S1" s="54" t="s">
+      <c r="S1" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="T1" s="54" t="s">
+      <c r="T1" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="U1" s="54" t="s">
+      <c r="U1" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="V1" s="54" t="s">
+      <c r="V1" s="50" t="s">
         <v>85</v>
       </c>
       <c r="W1" s="7"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="55">
-        <v>0</v>
-      </c>
-      <c r="C2" s="55">
-        <v>0</v>
-      </c>
-      <c r="D2" s="55">
-        <v>0</v>
-      </c>
-      <c r="E2" s="55">
-        <v>0</v>
-      </c>
-      <c r="F2" s="55">
-        <v>0</v>
-      </c>
-      <c r="G2" s="55">
-        <v>0</v>
-      </c>
-      <c r="H2" s="55">
-        <v>0</v>
-      </c>
-      <c r="I2" s="55">
-        <v>0</v>
-      </c>
-      <c r="J2" s="55">
-        <v>0</v>
-      </c>
-      <c r="K2" s="55">
-        <v>0</v>
-      </c>
-      <c r="L2" s="55">
-        <v>0</v>
-      </c>
-      <c r="M2" s="55">
-        <v>0</v>
-      </c>
-      <c r="N2" s="55">
-        <v>0</v>
-      </c>
-      <c r="O2" s="55">
-        <v>0</v>
-      </c>
-      <c r="P2" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="55">
-        <v>0</v>
-      </c>
-      <c r="R2" s="55">
-        <v>0</v>
-      </c>
-      <c r="S2" s="55">
-        <v>0</v>
-      </c>
-      <c r="T2" s="55">
-        <v>0</v>
-      </c>
-      <c r="U2" s="55">
-        <v>0</v>
-      </c>
-      <c r="V2" s="55">
+      <c r="B2" s="51">
+        <v>0</v>
+      </c>
+      <c r="C2" s="51">
+        <v>0</v>
+      </c>
+      <c r="D2" s="51">
+        <v>0</v>
+      </c>
+      <c r="E2" s="51">
+        <v>0</v>
+      </c>
+      <c r="F2" s="51">
+        <v>0</v>
+      </c>
+      <c r="G2" s="51">
+        <v>0</v>
+      </c>
+      <c r="H2" s="51">
+        <v>0</v>
+      </c>
+      <c r="I2" s="51">
+        <v>0</v>
+      </c>
+      <c r="J2" s="51">
+        <v>0</v>
+      </c>
+      <c r="K2" s="51">
+        <v>0</v>
+      </c>
+      <c r="L2" s="51">
+        <v>0</v>
+      </c>
+      <c r="M2" s="51">
+        <v>0</v>
+      </c>
+      <c r="N2" s="51">
+        <v>0</v>
+      </c>
+      <c r="O2" s="51">
+        <v>0</v>
+      </c>
+      <c r="P2" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="51">
+        <v>0</v>
+      </c>
+      <c r="R2" s="51">
+        <v>0</v>
+      </c>
+      <c r="S2" s="51">
+        <v>0</v>
+      </c>
+      <c r="T2" s="51">
+        <v>0</v>
+      </c>
+      <c r="U2" s="51">
+        <v>0</v>
+      </c>
+      <c r="V2" s="51">
         <v>0</v>
       </c>
       <c r="W2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A3" s="56" t="s">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="55">
-        <v>0</v>
-      </c>
-      <c r="C3" s="57">
+      <c r="B3" s="51">
+        <v>0</v>
+      </c>
+      <c r="C3" s="52">
         <f>'Data from BFPIaE'!E6/'Data from BFPIaE'!C6</f>
         <v>0.19493335993319316</v>
       </c>
-      <c r="D3" s="58">
-        <v>0</v>
-      </c>
-      <c r="E3" s="58">
-        <v>0</v>
-      </c>
-      <c r="F3" s="55">
-        <v>0</v>
-      </c>
-      <c r="G3" s="55">
-        <v>0</v>
-      </c>
-      <c r="H3" s="55">
-        <v>0</v>
-      </c>
-      <c r="I3" s="58">
-        <v>0</v>
-      </c>
-      <c r="J3" s="58">
-        <v>0</v>
-      </c>
-      <c r="K3" s="58">
-        <v>0</v>
-      </c>
-      <c r="L3" s="58">
-        <v>0</v>
-      </c>
-      <c r="M3" s="58">
-        <v>0</v>
-      </c>
-      <c r="N3" s="58">
-        <v>0</v>
-      </c>
-      <c r="O3" s="55">
-        <v>0</v>
-      </c>
-      <c r="P3" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="58">
-        <v>0</v>
-      </c>
-      <c r="R3" s="58">
-        <v>0</v>
-      </c>
-      <c r="S3" s="58">
-        <v>0</v>
-      </c>
-      <c r="T3" s="58">
-        <v>0</v>
-      </c>
-      <c r="U3" s="58">
-        <v>0</v>
-      </c>
-      <c r="V3" s="58">
+      <c r="D3" s="44">
+        <v>0</v>
+      </c>
+      <c r="E3" s="44">
+        <v>0</v>
+      </c>
+      <c r="F3" s="51">
+        <v>0</v>
+      </c>
+      <c r="G3" s="51">
+        <v>0</v>
+      </c>
+      <c r="H3" s="51">
+        <v>0</v>
+      </c>
+      <c r="I3" s="44">
+        <v>0</v>
+      </c>
+      <c r="J3" s="44">
+        <v>0</v>
+      </c>
+      <c r="K3" s="44">
+        <v>0</v>
+      </c>
+      <c r="L3" s="44">
+        <v>0</v>
+      </c>
+      <c r="M3" s="44">
+        <v>0</v>
+      </c>
+      <c r="N3" s="44">
+        <v>0</v>
+      </c>
+      <c r="O3" s="51">
+        <v>0</v>
+      </c>
+      <c r="P3" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="44">
+        <v>0</v>
+      </c>
+      <c r="R3" s="44">
+        <v>0</v>
+      </c>
+      <c r="S3" s="44">
+        <v>0</v>
+      </c>
+      <c r="T3" s="44">
+        <v>0</v>
+      </c>
+      <c r="U3" s="44">
+        <v>0</v>
+      </c>
+      <c r="V3" s="44">
         <v>0</v>
       </c>
       <c r="W3" s="7"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A4" s="56" t="s">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="55">
-        <v>0</v>
-      </c>
-      <c r="C4" s="58">
-        <v>0</v>
-      </c>
-      <c r="D4" s="57">
-        <f>'Data from BFPIaE'!E7/'Data from BFPIaE'!C7</f>
-        <v>0.71021923377833196</v>
-      </c>
-      <c r="E4" s="58">
-        <v>0</v>
-      </c>
-      <c r="F4" s="55">
-        <v>0</v>
-      </c>
-      <c r="G4" s="55">
-        <v>0</v>
-      </c>
-      <c r="H4" s="55">
-        <v>0</v>
-      </c>
-      <c r="I4" s="58">
-        <v>0</v>
-      </c>
-      <c r="J4" s="58">
-        <v>0</v>
-      </c>
-      <c r="K4" s="58">
-        <v>0</v>
-      </c>
-      <c r="L4" s="58">
-        <v>0</v>
-      </c>
-      <c r="M4" s="58">
-        <v>0</v>
-      </c>
-      <c r="N4" s="58">
-        <v>0</v>
-      </c>
-      <c r="O4" s="55">
-        <v>0</v>
-      </c>
-      <c r="P4" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="58">
-        <v>0</v>
-      </c>
-      <c r="R4" s="58">
-        <v>0</v>
-      </c>
-      <c r="S4" s="58">
-        <v>0</v>
-      </c>
-      <c r="T4" s="58">
-        <v>0</v>
-      </c>
-      <c r="U4" s="58">
-        <v>0</v>
-      </c>
-      <c r="V4" s="58">
+      <c r="B4" s="51">
+        <v>0</v>
+      </c>
+      <c r="C4" s="44">
+        <v>0</v>
+      </c>
+      <c r="D4" s="52">
+        <v>0</v>
+      </c>
+      <c r="E4" s="44">
+        <v>0</v>
+      </c>
+      <c r="F4" s="51">
+        <v>0</v>
+      </c>
+      <c r="G4" s="51">
+        <v>0</v>
+      </c>
+      <c r="H4" s="51">
+        <v>0</v>
+      </c>
+      <c r="I4" s="44">
+        <v>0</v>
+      </c>
+      <c r="J4" s="44">
+        <v>0</v>
+      </c>
+      <c r="K4" s="44">
+        <v>0</v>
+      </c>
+      <c r="L4" s="44">
+        <v>0</v>
+      </c>
+      <c r="M4" s="44">
+        <v>0</v>
+      </c>
+      <c r="N4" s="44">
+        <v>0</v>
+      </c>
+      <c r="O4" s="51">
+        <v>0</v>
+      </c>
+      <c r="P4" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="44">
+        <v>0</v>
+      </c>
+      <c r="R4" s="44">
+        <v>0</v>
+      </c>
+      <c r="S4" s="44">
+        <v>0</v>
+      </c>
+      <c r="T4" s="44">
+        <v>0</v>
+      </c>
+      <c r="U4" s="44">
+        <v>0</v>
+      </c>
+      <c r="V4" s="44">
         <v>0</v>
       </c>
       <c r="W4" s="7"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A5" s="56" t="s">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B5" s="55">
-        <v>0</v>
-      </c>
-      <c r="C5" s="58">
-        <v>0</v>
-      </c>
-      <c r="D5" s="58">
-        <v>0</v>
-      </c>
-      <c r="E5" s="57">
+      <c r="B5" s="51">
+        <v>0</v>
+      </c>
+      <c r="C5" s="44">
+        <v>0</v>
+      </c>
+      <c r="D5" s="44">
+        <v>0</v>
+      </c>
+      <c r="E5" s="52">
         <f>'Data from BFPIaE'!E8/'Data from BFPIaE'!C8</f>
         <v>0</v>
       </c>
-      <c r="F5" s="55">
-        <v>0</v>
-      </c>
-      <c r="G5" s="55">
-        <v>0</v>
-      </c>
-      <c r="H5" s="55">
-        <v>0</v>
-      </c>
-      <c r="I5" s="58">
-        <v>0</v>
-      </c>
-      <c r="J5" s="58">
-        <v>0</v>
-      </c>
-      <c r="K5" s="58">
-        <v>0</v>
-      </c>
-      <c r="L5" s="58">
-        <v>0</v>
-      </c>
-      <c r="M5" s="58">
-        <v>0</v>
-      </c>
-      <c r="N5" s="58">
-        <v>0</v>
-      </c>
-      <c r="O5" s="55">
-        <v>0</v>
-      </c>
-      <c r="P5" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="58">
-        <v>0</v>
-      </c>
-      <c r="R5" s="58">
-        <v>0</v>
-      </c>
-      <c r="S5" s="58">
-        <v>0</v>
-      </c>
-      <c r="T5" s="58">
-        <v>0</v>
-      </c>
-      <c r="U5" s="58">
-        <v>0</v>
-      </c>
-      <c r="V5" s="58">
+      <c r="F5" s="51">
+        <v>0</v>
+      </c>
+      <c r="G5" s="51">
+        <v>0</v>
+      </c>
+      <c r="H5" s="51">
+        <v>0</v>
+      </c>
+      <c r="I5" s="44">
+        <v>0</v>
+      </c>
+      <c r="J5" s="44">
+        <v>0</v>
+      </c>
+      <c r="K5" s="44">
+        <v>0</v>
+      </c>
+      <c r="L5" s="44">
+        <v>0</v>
+      </c>
+      <c r="M5" s="44">
+        <v>0</v>
+      </c>
+      <c r="N5" s="44">
+        <v>0</v>
+      </c>
+      <c r="O5" s="51">
+        <v>0</v>
+      </c>
+      <c r="P5" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="44">
+        <v>0</v>
+      </c>
+      <c r="R5" s="44">
+        <v>0</v>
+      </c>
+      <c r="S5" s="44">
+        <v>0</v>
+      </c>
+      <c r="T5" s="44">
+        <v>0</v>
+      </c>
+      <c r="U5" s="44">
+        <v>0</v>
+      </c>
+      <c r="V5" s="44">
         <v>0</v>
       </c>
       <c r="W5" s="7"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A6" s="59" t="s">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="55">
-        <v>0</v>
-      </c>
-      <c r="C6" s="55">
-        <v>0</v>
-      </c>
-      <c r="D6" s="55">
-        <v>0</v>
-      </c>
-      <c r="E6" s="55">
-        <v>0</v>
-      </c>
-      <c r="F6" s="55">
-        <v>0</v>
-      </c>
-      <c r="G6" s="55">
-        <v>0</v>
-      </c>
-      <c r="H6" s="55">
-        <v>0</v>
-      </c>
-      <c r="I6" s="55">
-        <v>0</v>
-      </c>
-      <c r="J6" s="55">
-        <v>0</v>
-      </c>
-      <c r="K6" s="55">
-        <v>0</v>
-      </c>
-      <c r="L6" s="55">
-        <v>0</v>
-      </c>
-      <c r="M6" s="55">
-        <v>0</v>
-      </c>
-      <c r="N6" s="55">
-        <v>0</v>
-      </c>
-      <c r="O6" s="55">
-        <v>0</v>
-      </c>
-      <c r="P6" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="55">
-        <v>0</v>
-      </c>
-      <c r="R6" s="55">
-        <v>0</v>
-      </c>
-      <c r="S6" s="55">
-        <v>0</v>
-      </c>
-      <c r="T6" s="55">
-        <v>0</v>
-      </c>
-      <c r="U6" s="55">
-        <v>0</v>
-      </c>
-      <c r="V6" s="55">
+      <c r="B6" s="51">
+        <v>0</v>
+      </c>
+      <c r="C6" s="51">
+        <v>0</v>
+      </c>
+      <c r="D6" s="51">
+        <v>0</v>
+      </c>
+      <c r="E6" s="51">
+        <v>0</v>
+      </c>
+      <c r="F6" s="51">
+        <v>0</v>
+      </c>
+      <c r="G6" s="51">
+        <v>0</v>
+      </c>
+      <c r="H6" s="51">
+        <v>0</v>
+      </c>
+      <c r="I6" s="51">
+        <v>0</v>
+      </c>
+      <c r="J6" s="51">
+        <v>0</v>
+      </c>
+      <c r="K6" s="51">
+        <v>0</v>
+      </c>
+      <c r="L6" s="51">
+        <v>0</v>
+      </c>
+      <c r="M6" s="51">
+        <v>0</v>
+      </c>
+      <c r="N6" s="51">
+        <v>0</v>
+      </c>
+      <c r="O6" s="51">
+        <v>0</v>
+      </c>
+      <c r="P6" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="51">
+        <v>0</v>
+      </c>
+      <c r="R6" s="51">
+        <v>0</v>
+      </c>
+      <c r="S6" s="51">
+        <v>0</v>
+      </c>
+      <c r="T6" s="51">
+        <v>0</v>
+      </c>
+      <c r="U6" s="51">
+        <v>0</v>
+      </c>
+      <c r="V6" s="51">
         <v>0</v>
       </c>
       <c r="W6" s="7"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A7" s="59" t="s">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="55">
-        <v>0</v>
-      </c>
-      <c r="C7" s="55">
-        <v>0</v>
-      </c>
-      <c r="D7" s="55">
-        <v>0</v>
-      </c>
-      <c r="E7" s="55">
-        <v>0</v>
-      </c>
-      <c r="F7" s="55">
-        <v>0</v>
-      </c>
-      <c r="G7" s="55">
-        <v>0</v>
-      </c>
-      <c r="H7" s="55">
-        <v>0</v>
-      </c>
-      <c r="I7" s="55">
-        <v>0</v>
-      </c>
-      <c r="J7" s="55">
-        <v>0</v>
-      </c>
-      <c r="K7" s="55">
-        <v>0</v>
-      </c>
-      <c r="L7" s="55">
-        <v>0</v>
-      </c>
-      <c r="M7" s="55">
-        <v>0</v>
-      </c>
-      <c r="N7" s="55">
-        <v>0</v>
-      </c>
-      <c r="O7" s="55">
-        <v>0</v>
-      </c>
-      <c r="P7" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="55">
-        <v>0</v>
-      </c>
-      <c r="R7" s="55">
-        <v>0</v>
-      </c>
-      <c r="S7" s="55">
-        <v>0</v>
-      </c>
-      <c r="T7" s="55">
-        <v>0</v>
-      </c>
-      <c r="U7" s="55">
-        <v>0</v>
-      </c>
-      <c r="V7" s="55">
+      <c r="B7" s="51">
+        <v>0</v>
+      </c>
+      <c r="C7" s="51">
+        <v>0</v>
+      </c>
+      <c r="D7" s="51">
+        <v>0</v>
+      </c>
+      <c r="E7" s="51">
+        <v>0</v>
+      </c>
+      <c r="F7" s="51">
+        <v>0</v>
+      </c>
+      <c r="G7" s="51">
+        <v>0</v>
+      </c>
+      <c r="H7" s="51">
+        <v>0</v>
+      </c>
+      <c r="I7" s="51">
+        <v>0</v>
+      </c>
+      <c r="J7" s="51">
+        <v>0</v>
+      </c>
+      <c r="K7" s="51">
+        <v>0</v>
+      </c>
+      <c r="L7" s="51">
+        <v>0</v>
+      </c>
+      <c r="M7" s="51">
+        <v>0</v>
+      </c>
+      <c r="N7" s="51">
+        <v>0</v>
+      </c>
+      <c r="O7" s="51">
+        <v>0</v>
+      </c>
+      <c r="P7" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="51">
+        <v>0</v>
+      </c>
+      <c r="R7" s="51">
+        <v>0</v>
+      </c>
+      <c r="S7" s="51">
+        <v>0</v>
+      </c>
+      <c r="T7" s="51">
+        <v>0</v>
+      </c>
+      <c r="U7" s="51">
+        <v>0</v>
+      </c>
+      <c r="V7" s="51">
         <v>0</v>
       </c>
       <c r="W7" s="7"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A8" s="59" t="s">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="B8" s="55">
-        <v>0</v>
-      </c>
-      <c r="C8" s="55">
-        <v>0</v>
-      </c>
-      <c r="D8" s="55">
-        <v>0</v>
-      </c>
-      <c r="E8" s="55">
-        <v>0</v>
-      </c>
-      <c r="F8" s="55">
-        <v>0</v>
-      </c>
-      <c r="G8" s="55">
-        <v>0</v>
-      </c>
-      <c r="H8" s="55">
-        <v>0</v>
-      </c>
-      <c r="I8" s="55">
-        <v>0</v>
-      </c>
-      <c r="J8" s="55">
-        <v>0</v>
-      </c>
-      <c r="K8" s="55">
-        <v>0</v>
-      </c>
-      <c r="L8" s="55">
-        <v>0</v>
-      </c>
-      <c r="M8" s="55">
-        <v>0</v>
-      </c>
-      <c r="N8" s="55">
-        <v>0</v>
-      </c>
-      <c r="O8" s="55">
-        <v>0</v>
-      </c>
-      <c r="P8" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="55">
-        <v>0</v>
-      </c>
-      <c r="R8" s="55">
-        <v>0</v>
-      </c>
-      <c r="S8" s="55">
-        <v>0</v>
-      </c>
-      <c r="T8" s="55">
-        <v>0</v>
-      </c>
-      <c r="U8" s="55">
-        <v>0</v>
-      </c>
-      <c r="V8" s="55">
+      <c r="B8" s="51">
+        <v>0</v>
+      </c>
+      <c r="C8" s="51">
+        <v>0</v>
+      </c>
+      <c r="D8" s="51">
+        <v>0</v>
+      </c>
+      <c r="E8" s="51">
+        <v>0</v>
+      </c>
+      <c r="F8" s="51">
+        <v>0</v>
+      </c>
+      <c r="G8" s="51">
+        <v>0</v>
+      </c>
+      <c r="H8" s="51">
+        <v>0</v>
+      </c>
+      <c r="I8" s="51">
+        <v>0</v>
+      </c>
+      <c r="J8" s="51">
+        <v>0</v>
+      </c>
+      <c r="K8" s="51">
+        <v>0</v>
+      </c>
+      <c r="L8" s="51">
+        <v>0</v>
+      </c>
+      <c r="M8" s="51">
+        <v>0</v>
+      </c>
+      <c r="N8" s="51">
+        <v>0</v>
+      </c>
+      <c r="O8" s="51">
+        <v>0</v>
+      </c>
+      <c r="P8" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="51">
+        <v>0</v>
+      </c>
+      <c r="R8" s="51">
+        <v>0</v>
+      </c>
+      <c r="S8" s="51">
+        <v>0</v>
+      </c>
+      <c r="T8" s="51">
+        <v>0</v>
+      </c>
+      <c r="U8" s="51">
+        <v>0</v>
+      </c>
+      <c r="V8" s="51">
         <v>0</v>
       </c>
       <c r="W8" s="7"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A9" s="56" t="s">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="55">
-        <v>0</v>
-      </c>
-      <c r="C9" s="58">
-        <v>0</v>
-      </c>
-      <c r="D9" s="58">
-        <v>0</v>
-      </c>
-      <c r="E9" s="58">
-        <v>0</v>
-      </c>
-      <c r="F9" s="55">
-        <v>0</v>
-      </c>
-      <c r="G9" s="55">
-        <v>0</v>
-      </c>
-      <c r="H9" s="55">
-        <v>0</v>
-      </c>
-      <c r="I9" s="57">
+      <c r="B9" s="51">
+        <v>0</v>
+      </c>
+      <c r="C9" s="44">
+        <v>0</v>
+      </c>
+      <c r="D9" s="44">
+        <v>0</v>
+      </c>
+      <c r="E9" s="44">
+        <v>0</v>
+      </c>
+      <c r="F9" s="51">
+        <v>0</v>
+      </c>
+      <c r="G9" s="51">
+        <v>0</v>
+      </c>
+      <c r="H9" s="51">
+        <v>0</v>
+      </c>
+      <c r="I9" s="52">
         <f>'Data from BFPIaE'!E12/'Data from BFPIaE'!C12</f>
         <v>4.8776638574552791E-2</v>
       </c>
-      <c r="J9" s="58">
-        <v>0</v>
-      </c>
-      <c r="K9" s="58">
-        <v>0</v>
-      </c>
-      <c r="L9" s="58">
-        <v>0</v>
-      </c>
-      <c r="M9" s="58">
-        <v>0</v>
-      </c>
-      <c r="N9" s="58">
-        <v>0</v>
-      </c>
-      <c r="O9" s="55">
-        <v>0</v>
-      </c>
-      <c r="P9" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="58">
-        <v>0</v>
-      </c>
-      <c r="R9" s="58">
-        <v>0</v>
-      </c>
-      <c r="S9" s="58">
-        <v>0</v>
-      </c>
-      <c r="T9" s="58">
-        <v>0</v>
-      </c>
-      <c r="U9" s="58">
-        <v>0</v>
-      </c>
-      <c r="V9" s="58">
+      <c r="J9" s="44">
+        <v>0</v>
+      </c>
+      <c r="K9" s="44">
+        <v>0</v>
+      </c>
+      <c r="L9" s="44">
+        <v>0</v>
+      </c>
+      <c r="M9" s="44">
+        <v>0</v>
+      </c>
+      <c r="N9" s="44">
+        <v>0</v>
+      </c>
+      <c r="O9" s="51">
+        <v>0</v>
+      </c>
+      <c r="P9" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="44">
+        <v>0</v>
+      </c>
+      <c r="R9" s="44">
+        <v>0</v>
+      </c>
+      <c r="S9" s="44">
+        <v>0</v>
+      </c>
+      <c r="T9" s="44">
+        <v>0</v>
+      </c>
+      <c r="U9" s="44">
+        <v>0</v>
+      </c>
+      <c r="V9" s="44">
         <v>0</v>
       </c>
       <c r="W9" s="7"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A10" s="56" t="s">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="55">
-        <v>0</v>
-      </c>
-      <c r="C10" s="58">
-        <v>0</v>
-      </c>
-      <c r="D10" s="58">
-        <v>0</v>
-      </c>
-      <c r="E10" s="58">
-        <v>0</v>
-      </c>
-      <c r="F10" s="55">
-        <v>0</v>
-      </c>
-      <c r="G10" s="55">
-        <v>0</v>
-      </c>
-      <c r="H10" s="55">
-        <v>0</v>
-      </c>
-      <c r="I10" s="58">
-        <v>0</v>
-      </c>
-      <c r="J10" s="60">
+      <c r="B10" s="51">
+        <v>0</v>
+      </c>
+      <c r="C10" s="44">
+        <v>0</v>
+      </c>
+      <c r="D10" s="44">
+        <v>0</v>
+      </c>
+      <c r="E10" s="44">
+        <v>0</v>
+      </c>
+      <c r="F10" s="51">
+        <v>0</v>
+      </c>
+      <c r="G10" s="51">
+        <v>0</v>
+      </c>
+      <c r="H10" s="51">
+        <v>0</v>
+      </c>
+      <c r="I10" s="44">
+        <v>0</v>
+      </c>
+      <c r="J10" s="54">
         <f>'Data from BFPIaE'!E13/SUM('Data from BFPIaE'!E13:F13)</f>
         <v>0.60771663482963756</v>
       </c>
-      <c r="K10" s="58">
-        <v>0</v>
-      </c>
-      <c r="L10" s="58">
-        <v>0</v>
-      </c>
-      <c r="M10" s="58">
-        <v>0</v>
-      </c>
-      <c r="N10" s="58">
-        <v>0</v>
-      </c>
-      <c r="O10" s="55">
-        <v>0</v>
-      </c>
-      <c r="P10" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="58">
-        <v>0</v>
-      </c>
-      <c r="R10" s="61">
+      <c r="K10" s="44">
+        <v>0</v>
+      </c>
+      <c r="L10" s="44">
+        <v>0</v>
+      </c>
+      <c r="M10" s="44">
+        <v>0</v>
+      </c>
+      <c r="N10" s="44">
+        <v>0</v>
+      </c>
+      <c r="O10" s="51">
+        <v>0</v>
+      </c>
+      <c r="P10" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="44">
+        <v>0</v>
+      </c>
+      <c r="R10" s="55">
         <f>1-J10</f>
         <v>0.39228336517036244</v>
       </c>
-      <c r="S10" s="58">
-        <v>0</v>
-      </c>
-      <c r="T10" s="58">
-        <v>0</v>
-      </c>
-      <c r="U10" s="58">
-        <v>0</v>
-      </c>
-      <c r="V10" s="58">
+      <c r="S10" s="44">
+        <v>0</v>
+      </c>
+      <c r="T10" s="44">
+        <v>0</v>
+      </c>
+      <c r="U10" s="44">
+        <v>0</v>
+      </c>
+      <c r="V10" s="44">
         <v>0</v>
       </c>
       <c r="W10" s="7"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A11" s="56" t="s">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B11" s="55">
-        <v>0</v>
-      </c>
-      <c r="C11" s="58">
-        <v>0</v>
-      </c>
-      <c r="D11" s="58">
-        <v>0</v>
-      </c>
-      <c r="E11" s="58">
-        <v>0</v>
-      </c>
-      <c r="F11" s="55">
-        <v>0</v>
-      </c>
-      <c r="G11" s="55">
-        <v>0</v>
-      </c>
-      <c r="H11" s="55">
-        <v>0</v>
-      </c>
-      <c r="I11" s="58">
-        <v>0</v>
-      </c>
-      <c r="J11" s="58">
-        <v>0</v>
-      </c>
-      <c r="K11" s="60">
+      <c r="B11" s="51">
+        <v>0</v>
+      </c>
+      <c r="C11" s="44">
+        <v>0</v>
+      </c>
+      <c r="D11" s="44">
+        <v>0</v>
+      </c>
+      <c r="E11" s="44">
+        <v>0</v>
+      </c>
+      <c r="F11" s="51">
+        <v>0</v>
+      </c>
+      <c r="G11" s="51">
+        <v>0</v>
+      </c>
+      <c r="H11" s="51">
+        <v>0</v>
+      </c>
+      <c r="I11" s="44">
+        <v>0</v>
+      </c>
+      <c r="J11" s="44">
+        <v>0</v>
+      </c>
+      <c r="K11" s="54">
         <f>'Data from BFPIaE'!E14/SUM('Data from BFPIaE'!E14:F14)</f>
         <v>0.29449515789635189</v>
       </c>
-      <c r="L11" s="58">
-        <v>0</v>
-      </c>
-      <c r="M11" s="58">
-        <v>0</v>
-      </c>
-      <c r="N11" s="58">
-        <v>0</v>
-      </c>
-      <c r="O11" s="55">
-        <v>0</v>
-      </c>
-      <c r="P11" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="58">
-        <v>0</v>
-      </c>
-      <c r="R11" s="61">
+      <c r="L11" s="44">
+        <v>0</v>
+      </c>
+      <c r="M11" s="44">
+        <v>0</v>
+      </c>
+      <c r="N11" s="44">
+        <v>0</v>
+      </c>
+      <c r="O11" s="51">
+        <v>0</v>
+      </c>
+      <c r="P11" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="44">
+        <v>0</v>
+      </c>
+      <c r="R11" s="55">
         <f>1-K11</f>
         <v>0.70550484210364806</v>
       </c>
-      <c r="S11" s="58">
-        <v>0</v>
-      </c>
-      <c r="T11" s="58">
-        <v>0</v>
-      </c>
-      <c r="U11" s="58">
-        <v>0</v>
-      </c>
-      <c r="V11" s="58">
+      <c r="S11" s="44">
+        <v>0</v>
+      </c>
+      <c r="T11" s="44">
+        <v>0</v>
+      </c>
+      <c r="U11" s="44">
+        <v>0</v>
+      </c>
+      <c r="V11" s="44">
         <v>0</v>
       </c>
       <c r="W11" s="7"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A12" s="56" t="s">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="55">
-        <v>0</v>
-      </c>
-      <c r="C12" s="58">
-        <v>0</v>
-      </c>
-      <c r="D12" s="58">
-        <v>0</v>
-      </c>
-      <c r="E12" s="58">
-        <v>0</v>
-      </c>
-      <c r="F12" s="55">
-        <v>0</v>
-      </c>
-      <c r="G12" s="55">
-        <v>0</v>
-      </c>
-      <c r="H12" s="55">
-        <v>0</v>
-      </c>
-      <c r="I12" s="58">
-        <v>0</v>
-      </c>
-      <c r="J12" s="58">
-        <v>0</v>
-      </c>
-      <c r="K12" s="58">
-        <v>0</v>
-      </c>
-      <c r="L12" s="57">
+      <c r="B12" s="51">
+        <v>0</v>
+      </c>
+      <c r="C12" s="44">
+        <v>0</v>
+      </c>
+      <c r="D12" s="44">
+        <v>0</v>
+      </c>
+      <c r="E12" s="44">
+        <v>0</v>
+      </c>
+      <c r="F12" s="51">
+        <v>0</v>
+      </c>
+      <c r="G12" s="51">
+        <v>0</v>
+      </c>
+      <c r="H12" s="51">
+        <v>0</v>
+      </c>
+      <c r="I12" s="44">
+        <v>0</v>
+      </c>
+      <c r="J12" s="44">
+        <v>0</v>
+      </c>
+      <c r="K12" s="44">
+        <v>0</v>
+      </c>
+      <c r="L12" s="52">
         <f>'Data from BFPIaE'!E15/'Data from BFPIaE'!C15</f>
         <v>0.50956274490095177</v>
       </c>
-      <c r="M12" s="58">
-        <v>0</v>
-      </c>
-      <c r="N12" s="58">
-        <v>0</v>
-      </c>
-      <c r="O12" s="55">
-        <v>0</v>
-      </c>
-      <c r="P12" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="58">
-        <v>0</v>
-      </c>
-      <c r="R12" s="58">
-        <v>0</v>
-      </c>
-      <c r="S12" s="58">
-        <v>0</v>
-      </c>
-      <c r="T12" s="58">
-        <v>0</v>
-      </c>
-      <c r="U12" s="58">
-        <v>0</v>
-      </c>
-      <c r="V12" s="58">
+      <c r="M12" s="44">
+        <v>0</v>
+      </c>
+      <c r="N12" s="44">
+        <v>0</v>
+      </c>
+      <c r="O12" s="51">
+        <v>0</v>
+      </c>
+      <c r="P12" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="44">
+        <v>0</v>
+      </c>
+      <c r="R12" s="44">
+        <v>0</v>
+      </c>
+      <c r="S12" s="44">
+        <v>0</v>
+      </c>
+      <c r="T12" s="44">
+        <v>0</v>
+      </c>
+      <c r="U12" s="44">
+        <v>0</v>
+      </c>
+      <c r="V12" s="44">
         <v>0</v>
       </c>
       <c r="W12" s="7"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A13" s="56" t="s">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B13" s="55">
-        <v>0</v>
-      </c>
-      <c r="C13" s="58">
-        <v>0</v>
-      </c>
-      <c r="D13" s="58">
-        <v>0</v>
-      </c>
-      <c r="E13" s="58">
-        <v>0</v>
-      </c>
-      <c r="F13" s="55">
-        <v>0</v>
-      </c>
-      <c r="G13" s="55">
-        <v>0</v>
-      </c>
-      <c r="H13" s="55">
-        <v>0</v>
-      </c>
-      <c r="I13" s="58">
-        <v>0</v>
-      </c>
-      <c r="J13" s="58">
-        <v>0</v>
-      </c>
-      <c r="K13" s="58">
-        <v>0</v>
-      </c>
-      <c r="L13" s="58">
-        <v>0</v>
-      </c>
-      <c r="M13" s="57">
+      <c r="B13" s="51">
+        <v>0</v>
+      </c>
+      <c r="C13" s="44">
+        <v>0</v>
+      </c>
+      <c r="D13" s="44">
+        <v>0</v>
+      </c>
+      <c r="E13" s="44">
+        <v>0</v>
+      </c>
+      <c r="F13" s="51">
+        <v>0</v>
+      </c>
+      <c r="G13" s="51">
+        <v>0</v>
+      </c>
+      <c r="H13" s="51">
+        <v>0</v>
+      </c>
+      <c r="I13" s="44">
+        <v>0</v>
+      </c>
+      <c r="J13" s="44">
+        <v>0</v>
+      </c>
+      <c r="K13" s="44">
+        <v>0</v>
+      </c>
+      <c r="L13" s="44">
+        <v>0</v>
+      </c>
+      <c r="M13" s="52">
         <f>'Data from BFPIaE'!E16/'Data from BFPIaE'!C16</f>
         <v>0.66157955210681685</v>
       </c>
-      <c r="N13" s="58">
-        <v>0</v>
-      </c>
-      <c r="O13" s="55">
-        <v>0</v>
-      </c>
-      <c r="P13" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="58">
-        <v>0</v>
-      </c>
-      <c r="R13" s="58">
-        <v>0</v>
-      </c>
-      <c r="S13" s="58">
-        <v>0</v>
-      </c>
-      <c r="T13" s="58">
-        <v>0</v>
-      </c>
-      <c r="U13" s="58">
-        <v>0</v>
-      </c>
-      <c r="V13" s="58">
+      <c r="N13" s="44">
+        <v>0</v>
+      </c>
+      <c r="O13" s="51">
+        <v>0</v>
+      </c>
+      <c r="P13" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="44">
+        <v>0</v>
+      </c>
+      <c r="R13" s="44">
+        <v>0</v>
+      </c>
+      <c r="S13" s="44">
+        <v>0</v>
+      </c>
+      <c r="T13" s="44">
+        <v>0</v>
+      </c>
+      <c r="U13" s="44">
+        <v>0</v>
+      </c>
+      <c r="V13" s="44">
         <v>0</v>
       </c>
       <c r="W13" s="7"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A14" s="56" t="s">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="55">
-        <v>0</v>
-      </c>
-      <c r="C14" s="58">
-        <v>0</v>
-      </c>
-      <c r="D14" s="58">
-        <v>0</v>
-      </c>
-      <c r="E14" s="58">
-        <v>0</v>
-      </c>
-      <c r="F14" s="55">
-        <v>0</v>
-      </c>
-      <c r="G14" s="55">
-        <v>0</v>
-      </c>
-      <c r="H14" s="55">
-        <v>0</v>
-      </c>
-      <c r="I14" s="58">
-        <v>0</v>
-      </c>
-      <c r="J14" s="58">
-        <v>0</v>
-      </c>
-      <c r="K14" s="58">
-        <v>0</v>
-      </c>
-      <c r="L14" s="58">
-        <v>0</v>
-      </c>
-      <c r="M14" s="58">
-        <v>0</v>
-      </c>
-      <c r="N14" s="60">
+      <c r="B14" s="51">
+        <v>0</v>
+      </c>
+      <c r="C14" s="44">
+        <v>0</v>
+      </c>
+      <c r="D14" s="44">
+        <v>0</v>
+      </c>
+      <c r="E14" s="44">
+        <v>0</v>
+      </c>
+      <c r="F14" s="51">
+        <v>0</v>
+      </c>
+      <c r="G14" s="51">
+        <v>0</v>
+      </c>
+      <c r="H14" s="51">
+        <v>0</v>
+      </c>
+      <c r="I14" s="44">
+        <v>0</v>
+      </c>
+      <c r="J14" s="44">
+        <v>0</v>
+      </c>
+      <c r="K14" s="44">
+        <v>0</v>
+      </c>
+      <c r="L14" s="44">
+        <v>0</v>
+      </c>
+      <c r="M14" s="44">
+        <v>0</v>
+      </c>
+      <c r="N14" s="54">
         <f>'Data from BFPIaE'!E17/SUM('Data from BFPIaE'!E17:F17)</f>
         <v>0.27913977313035632</v>
       </c>
-      <c r="O14" s="55">
-        <v>0</v>
-      </c>
-      <c r="P14" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="58">
-        <v>0</v>
-      </c>
-      <c r="R14" s="61">
+      <c r="O14" s="51">
+        <v>0</v>
+      </c>
+      <c r="P14" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="44">
+        <v>0</v>
+      </c>
+      <c r="R14" s="55">
         <f>1-N14</f>
         <v>0.72086022686964368</v>
       </c>
-      <c r="S14" s="58">
-        <v>0</v>
-      </c>
-      <c r="T14" s="58">
-        <v>0</v>
-      </c>
-      <c r="U14" s="58">
-        <v>0</v>
-      </c>
-      <c r="V14" s="58">
+      <c r="S14" s="44">
+        <v>0</v>
+      </c>
+      <c r="T14" s="44">
+        <v>0</v>
+      </c>
+      <c r="U14" s="44">
+        <v>0</v>
+      </c>
+      <c r="V14" s="44">
         <v>0</v>
       </c>
       <c r="W14" s="7"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A15" s="59" t="s">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="55">
-        <v>0</v>
-      </c>
-      <c r="C15" s="55">
-        <v>0</v>
-      </c>
-      <c r="D15" s="55">
-        <v>0</v>
-      </c>
-      <c r="E15" s="55">
-        <v>0</v>
-      </c>
-      <c r="F15" s="55">
-        <v>0</v>
-      </c>
-      <c r="G15" s="55">
-        <v>0</v>
-      </c>
-      <c r="H15" s="55">
-        <v>0</v>
-      </c>
-      <c r="I15" s="55">
-        <v>0</v>
-      </c>
-      <c r="J15" s="55">
-        <v>0</v>
-      </c>
-      <c r="K15" s="55">
-        <v>0</v>
-      </c>
-      <c r="L15" s="55">
-        <v>0</v>
-      </c>
-      <c r="M15" s="55">
-        <v>0</v>
-      </c>
-      <c r="N15" s="55">
-        <v>0</v>
-      </c>
-      <c r="O15" s="55">
-        <v>0</v>
-      </c>
-      <c r="P15" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="55">
-        <v>0</v>
-      </c>
-      <c r="R15" s="55">
-        <v>0</v>
-      </c>
-      <c r="S15" s="55">
-        <v>0</v>
-      </c>
-      <c r="T15" s="55">
-        <v>0</v>
-      </c>
-      <c r="U15" s="55">
-        <v>0</v>
-      </c>
-      <c r="V15" s="55">
+      <c r="B15" s="51">
+        <v>0</v>
+      </c>
+      <c r="C15" s="51">
+        <v>0</v>
+      </c>
+      <c r="D15" s="51">
+        <v>0</v>
+      </c>
+      <c r="E15" s="51">
+        <v>0</v>
+      </c>
+      <c r="F15" s="51">
+        <v>0</v>
+      </c>
+      <c r="G15" s="51">
+        <v>0</v>
+      </c>
+      <c r="H15" s="51">
+        <v>0</v>
+      </c>
+      <c r="I15" s="51">
+        <v>0</v>
+      </c>
+      <c r="J15" s="51">
+        <v>0</v>
+      </c>
+      <c r="K15" s="51">
+        <v>0</v>
+      </c>
+      <c r="L15" s="51">
+        <v>0</v>
+      </c>
+      <c r="M15" s="51">
+        <v>0</v>
+      </c>
+      <c r="N15" s="51">
+        <v>0</v>
+      </c>
+      <c r="O15" s="51">
+        <v>0</v>
+      </c>
+      <c r="P15" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="51">
+        <v>0</v>
+      </c>
+      <c r="R15" s="51">
+        <v>0</v>
+      </c>
+      <c r="S15" s="51">
+        <v>0</v>
+      </c>
+      <c r="T15" s="51">
+        <v>0</v>
+      </c>
+      <c r="U15" s="51">
+        <v>0</v>
+      </c>
+      <c r="V15" s="51">
         <v>0</v>
       </c>
       <c r="W15" s="7"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A16" s="59" t="s">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="B16" s="55">
-        <v>0</v>
-      </c>
-      <c r="C16" s="55">
-        <v>0</v>
-      </c>
-      <c r="D16" s="55">
-        <v>0</v>
-      </c>
-      <c r="E16" s="55">
-        <v>0</v>
-      </c>
-      <c r="F16" s="55">
-        <v>0</v>
-      </c>
-      <c r="G16" s="55">
-        <v>0</v>
-      </c>
-      <c r="H16" s="55">
-        <v>0</v>
-      </c>
-      <c r="I16" s="55">
-        <v>0</v>
-      </c>
-      <c r="J16" s="55">
-        <v>0</v>
-      </c>
-      <c r="K16" s="55">
-        <v>0</v>
-      </c>
-      <c r="L16" s="55">
-        <v>0</v>
-      </c>
-      <c r="M16" s="55">
-        <v>0</v>
-      </c>
-      <c r="N16" s="55">
-        <v>0</v>
-      </c>
-      <c r="O16" s="55">
-        <v>0</v>
-      </c>
-      <c r="P16" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="55">
-        <v>0</v>
-      </c>
-      <c r="R16" s="55">
-        <v>0</v>
-      </c>
-      <c r="S16" s="55">
-        <v>0</v>
-      </c>
-      <c r="T16" s="55">
-        <v>0</v>
-      </c>
-      <c r="U16" s="55">
-        <v>0</v>
-      </c>
-      <c r="V16" s="55">
+      <c r="B16" s="51">
+        <v>0</v>
+      </c>
+      <c r="C16" s="51">
+        <v>0</v>
+      </c>
+      <c r="D16" s="51">
+        <v>0</v>
+      </c>
+      <c r="E16" s="51">
+        <v>0</v>
+      </c>
+      <c r="F16" s="51">
+        <v>0</v>
+      </c>
+      <c r="G16" s="51">
+        <v>0</v>
+      </c>
+      <c r="H16" s="51">
+        <v>0</v>
+      </c>
+      <c r="I16" s="51">
+        <v>0</v>
+      </c>
+      <c r="J16" s="51">
+        <v>0</v>
+      </c>
+      <c r="K16" s="51">
+        <v>0</v>
+      </c>
+      <c r="L16" s="51">
+        <v>0</v>
+      </c>
+      <c r="M16" s="51">
+        <v>0</v>
+      </c>
+      <c r="N16" s="51">
+        <v>0</v>
+      </c>
+      <c r="O16" s="51">
+        <v>0</v>
+      </c>
+      <c r="P16" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="51">
+        <v>0</v>
+      </c>
+      <c r="R16" s="51">
+        <v>0</v>
+      </c>
+      <c r="S16" s="51">
+        <v>0</v>
+      </c>
+      <c r="T16" s="51">
+        <v>0</v>
+      </c>
+      <c r="U16" s="51">
+        <v>0</v>
+      </c>
+      <c r="V16" s="51">
         <v>0</v>
       </c>
       <c r="W16" s="7"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A17" s="56" t="s">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B17" s="55">
-        <v>0</v>
-      </c>
-      <c r="C17" s="58">
-        <v>0</v>
-      </c>
-      <c r="D17" s="58">
-        <v>0</v>
-      </c>
-      <c r="E17" s="58">
-        <v>0</v>
-      </c>
-      <c r="F17" s="55">
-        <v>0</v>
-      </c>
-      <c r="G17" s="55">
-        <v>0</v>
-      </c>
-      <c r="H17" s="55">
-        <v>0</v>
-      </c>
-      <c r="I17" s="58">
-        <v>0</v>
-      </c>
-      <c r="J17" s="58">
-        <v>0</v>
-      </c>
-      <c r="K17" s="58">
-        <v>0</v>
-      </c>
-      <c r="L17" s="58">
-        <v>0</v>
-      </c>
-      <c r="M17" s="58">
-        <v>0</v>
-      </c>
-      <c r="N17" s="58">
-        <v>0</v>
-      </c>
-      <c r="O17" s="55">
-        <v>0</v>
-      </c>
-      <c r="P17" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="62">
+      <c r="B17" s="51">
+        <v>0</v>
+      </c>
+      <c r="C17" s="44">
+        <v>0</v>
+      </c>
+      <c r="D17" s="44">
+        <v>0</v>
+      </c>
+      <c r="E17" s="44">
+        <v>0</v>
+      </c>
+      <c r="F17" s="51">
+        <v>0</v>
+      </c>
+      <c r="G17" s="51">
+        <v>0</v>
+      </c>
+      <c r="H17" s="51">
+        <v>0</v>
+      </c>
+      <c r="I17" s="44">
+        <v>0</v>
+      </c>
+      <c r="J17" s="44">
+        <v>0</v>
+      </c>
+      <c r="K17" s="44">
+        <v>0</v>
+      </c>
+      <c r="L17" s="44">
+        <v>0</v>
+      </c>
+      <c r="M17" s="44">
+        <v>0</v>
+      </c>
+      <c r="N17" s="44">
+        <v>0</v>
+      </c>
+      <c r="O17" s="51">
+        <v>0</v>
+      </c>
+      <c r="P17" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="56">
         <f>'Data from BFPIaE'!E20/'Data from BFPIaE'!C20</f>
         <v>0.13327901247089191</v>
       </c>
-      <c r="R17" s="58">
-        <v>0</v>
-      </c>
-      <c r="S17" s="58">
-        <v>0</v>
-      </c>
-      <c r="T17" s="58">
-        <v>0</v>
-      </c>
-      <c r="U17" s="58">
-        <v>0</v>
-      </c>
-      <c r="V17" s="58">
+      <c r="R17" s="44">
+        <v>0</v>
+      </c>
+      <c r="S17" s="44">
+        <v>0</v>
+      </c>
+      <c r="T17" s="44">
+        <v>0</v>
+      </c>
+      <c r="U17" s="44">
+        <v>0</v>
+      </c>
+      <c r="V17" s="44">
         <v>0</v>
       </c>
       <c r="W17" s="7"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A18" s="56" t="s">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="55">
-        <v>0</v>
-      </c>
-      <c r="C18" s="58">
-        <v>0</v>
-      </c>
-      <c r="D18" s="58">
-        <v>0</v>
-      </c>
-      <c r="E18" s="58">
-        <v>0</v>
-      </c>
-      <c r="F18" s="55">
-        <v>0</v>
-      </c>
-      <c r="G18" s="55">
-        <v>0</v>
-      </c>
-      <c r="H18" s="55">
-        <v>0</v>
-      </c>
-      <c r="I18" s="58">
-        <v>0</v>
-      </c>
-      <c r="J18" s="58">
-        <v>0</v>
-      </c>
-      <c r="K18" s="58">
-        <v>0</v>
-      </c>
-      <c r="L18" s="58">
-        <v>0</v>
-      </c>
-      <c r="M18" s="58">
-        <v>0</v>
-      </c>
-      <c r="N18" s="58">
-        <v>0</v>
-      </c>
-      <c r="O18" s="55">
-        <v>0</v>
-      </c>
-      <c r="P18" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="58">
-        <v>0</v>
-      </c>
-      <c r="R18" s="60">
-        <v>1</v>
-      </c>
-      <c r="S18" s="58">
-        <v>0</v>
-      </c>
-      <c r="T18" s="58">
-        <v>0</v>
-      </c>
-      <c r="U18" s="58">
-        <v>0</v>
-      </c>
-      <c r="V18" s="58">
+      <c r="B18" s="51">
+        <v>0</v>
+      </c>
+      <c r="C18" s="44">
+        <v>0</v>
+      </c>
+      <c r="D18" s="44">
+        <v>0</v>
+      </c>
+      <c r="E18" s="44">
+        <v>0</v>
+      </c>
+      <c r="F18" s="51">
+        <v>0</v>
+      </c>
+      <c r="G18" s="51">
+        <v>0</v>
+      </c>
+      <c r="H18" s="51">
+        <v>0</v>
+      </c>
+      <c r="I18" s="44">
+        <v>0</v>
+      </c>
+      <c r="J18" s="44">
+        <v>0</v>
+      </c>
+      <c r="K18" s="44">
+        <v>0</v>
+      </c>
+      <c r="L18" s="44">
+        <v>0</v>
+      </c>
+      <c r="M18" s="44">
+        <v>0</v>
+      </c>
+      <c r="N18" s="44">
+        <v>0</v>
+      </c>
+      <c r="O18" s="51">
+        <v>0</v>
+      </c>
+      <c r="P18" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="44">
+        <v>0</v>
+      </c>
+      <c r="R18" s="54">
+        <v>0</v>
+      </c>
+      <c r="S18" s="44">
+        <v>0</v>
+      </c>
+      <c r="T18" s="44">
+        <v>0</v>
+      </c>
+      <c r="U18" s="44">
+        <v>0</v>
+      </c>
+      <c r="V18" s="44">
         <v>0</v>
       </c>
       <c r="W18" s="7"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A19" s="56" t="s">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B19" s="55">
-        <v>0</v>
-      </c>
-      <c r="C19" s="58">
-        <v>0</v>
-      </c>
-      <c r="D19" s="58">
-        <v>0</v>
-      </c>
-      <c r="E19" s="58">
-        <v>0</v>
-      </c>
-      <c r="F19" s="55">
-        <v>0</v>
-      </c>
-      <c r="G19" s="55">
-        <v>0</v>
-      </c>
-      <c r="H19" s="55">
-        <v>0</v>
-      </c>
-      <c r="I19" s="58">
-        <v>0</v>
-      </c>
-      <c r="J19" s="58">
-        <v>0</v>
-      </c>
-      <c r="K19" s="58">
-        <v>0</v>
-      </c>
-      <c r="L19" s="58">
-        <v>0</v>
-      </c>
-      <c r="M19" s="58">
-        <v>0</v>
-      </c>
-      <c r="N19" s="58">
-        <v>0</v>
-      </c>
-      <c r="O19" s="55">
-        <v>0</v>
-      </c>
-      <c r="P19" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="58">
-        <v>0</v>
-      </c>
-      <c r="R19" s="61">
+      <c r="B19" s="51">
+        <v>0</v>
+      </c>
+      <c r="C19" s="44">
+        <v>0</v>
+      </c>
+      <c r="D19" s="44">
+        <v>0</v>
+      </c>
+      <c r="E19" s="44">
+        <v>0</v>
+      </c>
+      <c r="F19" s="51">
+        <v>0</v>
+      </c>
+      <c r="G19" s="51">
+        <v>0</v>
+      </c>
+      <c r="H19" s="51">
+        <v>0</v>
+      </c>
+      <c r="I19" s="44">
+        <v>0</v>
+      </c>
+      <c r="J19" s="44">
+        <v>0</v>
+      </c>
+      <c r="K19" s="44">
+        <v>0</v>
+      </c>
+      <c r="L19" s="44">
+        <v>0</v>
+      </c>
+      <c r="M19" s="44">
+        <v>0</v>
+      </c>
+      <c r="N19" s="44">
+        <v>0</v>
+      </c>
+      <c r="O19" s="51">
+        <v>0</v>
+      </c>
+      <c r="P19" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="44">
+        <v>0</v>
+      </c>
+      <c r="R19" s="55">
         <f>1-S19</f>
         <v>0.49856575142985637</v>
       </c>
-      <c r="S19" s="60">
+      <c r="S19" s="54">
         <f>'Data from BFPIaE'!E22/SUM('Data from BFPIaE'!E22:F22)</f>
         <v>0.50143424857014363</v>
       </c>
-      <c r="T19" s="58">
-        <v>0</v>
-      </c>
-      <c r="U19" s="58">
-        <v>0</v>
-      </c>
-      <c r="V19" s="58">
+      <c r="T19" s="44">
+        <v>0</v>
+      </c>
+      <c r="U19" s="44">
+        <v>0</v>
+      </c>
+      <c r="V19" s="44">
         <v>0</v>
       </c>
       <c r="W19" s="7"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A20" s="56" t="s">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="55">
-        <v>0</v>
-      </c>
-      <c r="C20" s="58">
-        <v>0</v>
-      </c>
-      <c r="D20" s="58">
-        <v>0</v>
-      </c>
-      <c r="E20" s="58">
-        <v>0</v>
-      </c>
-      <c r="F20" s="55">
-        <v>0</v>
-      </c>
-      <c r="G20" s="55">
-        <v>0</v>
-      </c>
-      <c r="H20" s="55">
-        <v>0</v>
-      </c>
-      <c r="I20" s="58">
-        <v>0</v>
-      </c>
-      <c r="J20" s="58">
-        <v>0</v>
-      </c>
-      <c r="K20" s="58">
-        <v>0</v>
-      </c>
-      <c r="L20" s="58">
-        <v>0</v>
-      </c>
-      <c r="M20" s="58">
-        <v>0</v>
-      </c>
-      <c r="N20" s="58">
-        <v>0</v>
-      </c>
-      <c r="O20" s="55">
-        <v>0</v>
-      </c>
-      <c r="P20" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="58">
-        <v>0</v>
-      </c>
-      <c r="R20" s="61">
+      <c r="B20" s="51">
+        <v>0</v>
+      </c>
+      <c r="C20" s="44">
+        <v>0</v>
+      </c>
+      <c r="D20" s="44">
+        <v>0</v>
+      </c>
+      <c r="E20" s="44">
+        <v>0</v>
+      </c>
+      <c r="F20" s="51">
+        <v>0</v>
+      </c>
+      <c r="G20" s="51">
+        <v>0</v>
+      </c>
+      <c r="H20" s="51">
+        <v>0</v>
+      </c>
+      <c r="I20" s="44">
+        <v>0</v>
+      </c>
+      <c r="J20" s="44">
+        <v>0</v>
+      </c>
+      <c r="K20" s="44">
+        <v>0</v>
+      </c>
+      <c r="L20" s="44">
+        <v>0</v>
+      </c>
+      <c r="M20" s="44">
+        <v>0</v>
+      </c>
+      <c r="N20" s="44">
+        <v>0</v>
+      </c>
+      <c r="O20" s="51">
+        <v>0</v>
+      </c>
+      <c r="P20" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="44">
+        <v>0</v>
+      </c>
+      <c r="R20" s="55">
         <f>1-T20</f>
         <v>0.84498067686633227</v>
       </c>
-      <c r="S20" s="58">
-        <v>0</v>
-      </c>
-      <c r="T20" s="60">
+      <c r="S20" s="44">
+        <v>0</v>
+      </c>
+      <c r="T20" s="54">
         <f>'Data from BFPIaE'!E23/SUM('Data from BFPIaE'!E23:F23)</f>
         <v>0.15501932313366773</v>
       </c>
-      <c r="U20" s="58">
-        <v>0</v>
-      </c>
-      <c r="V20" s="58">
+      <c r="U20" s="44">
+        <v>0</v>
+      </c>
+      <c r="V20" s="44">
         <v>0</v>
       </c>
       <c r="W20" s="7"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A21" s="56" t="s">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="55">
-        <v>0</v>
-      </c>
-      <c r="C21" s="58">
-        <v>0</v>
-      </c>
-      <c r="D21" s="58">
-        <v>0</v>
-      </c>
-      <c r="E21" s="58">
-        <v>0</v>
-      </c>
-      <c r="F21" s="55">
-        <v>0</v>
-      </c>
-      <c r="G21" s="55">
-        <v>0</v>
-      </c>
-      <c r="H21" s="55">
-        <v>0</v>
-      </c>
-      <c r="I21" s="58">
-        <v>0</v>
-      </c>
-      <c r="J21" s="58">
-        <v>0</v>
-      </c>
-      <c r="K21" s="58">
-        <v>0</v>
-      </c>
-      <c r="L21" s="58">
-        <v>0</v>
-      </c>
-      <c r="M21" s="58">
-        <v>0</v>
-      </c>
-      <c r="N21" s="58">
-        <v>0</v>
-      </c>
-      <c r="O21" s="55">
-        <v>0</v>
-      </c>
-      <c r="P21" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="58">
-        <v>0</v>
-      </c>
-      <c r="R21" s="58">
-        <v>0</v>
-      </c>
-      <c r="S21" s="58">
-        <v>0</v>
-      </c>
-      <c r="T21" s="58">
-        <v>0</v>
-      </c>
-      <c r="U21" s="57">
+      <c r="B21" s="51">
+        <v>0</v>
+      </c>
+      <c r="C21" s="44">
+        <v>0</v>
+      </c>
+      <c r="D21" s="44">
+        <v>0</v>
+      </c>
+      <c r="E21" s="44">
+        <v>0</v>
+      </c>
+      <c r="F21" s="51">
+        <v>0</v>
+      </c>
+      <c r="G21" s="51">
+        <v>0</v>
+      </c>
+      <c r="H21" s="51">
+        <v>0</v>
+      </c>
+      <c r="I21" s="44">
+        <v>0</v>
+      </c>
+      <c r="J21" s="44">
+        <v>0</v>
+      </c>
+      <c r="K21" s="44">
+        <v>0</v>
+      </c>
+      <c r="L21" s="44">
+        <v>0</v>
+      </c>
+      <c r="M21" s="44">
+        <v>0</v>
+      </c>
+      <c r="N21" s="44">
+        <v>0</v>
+      </c>
+      <c r="O21" s="51">
+        <v>0</v>
+      </c>
+      <c r="P21" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="44">
+        <v>0</v>
+      </c>
+      <c r="R21" s="44">
+        <v>0</v>
+      </c>
+      <c r="S21" s="44">
+        <v>0</v>
+      </c>
+      <c r="T21" s="44">
+        <v>0</v>
+      </c>
+      <c r="U21" s="52">
         <f>'Data from BFPIaE'!E24/'Data from BFPIaE'!C24</f>
         <v>1.9088470132744644E-3</v>
       </c>
-      <c r="V21" s="58">
+      <c r="V21" s="44">
         <v>0</v>
       </c>
       <c r="W21" s="7"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A22" s="56" t="s">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="55">
-        <v>0</v>
-      </c>
-      <c r="C22" s="58">
-        <v>0</v>
-      </c>
-      <c r="D22" s="58">
-        <v>0</v>
-      </c>
-      <c r="E22" s="58">
-        <v>0</v>
-      </c>
-      <c r="F22" s="55">
-        <v>0</v>
-      </c>
-      <c r="G22" s="55">
-        <v>0</v>
-      </c>
-      <c r="H22" s="55">
-        <v>0</v>
-      </c>
-      <c r="I22" s="58">
-        <v>0</v>
-      </c>
-      <c r="J22" s="58">
-        <v>0</v>
-      </c>
-      <c r="K22" s="58">
-        <v>0</v>
-      </c>
-      <c r="L22" s="58">
-        <v>0</v>
-      </c>
-      <c r="M22" s="58">
-        <v>0</v>
-      </c>
-      <c r="N22" s="58">
-        <v>0</v>
-      </c>
-      <c r="O22" s="55">
-        <v>0</v>
-      </c>
-      <c r="P22" s="55">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="58">
-        <v>0</v>
-      </c>
-      <c r="R22" s="58">
-        <v>0</v>
-      </c>
-      <c r="S22" s="58">
-        <v>0</v>
-      </c>
-      <c r="T22" s="58">
-        <v>0</v>
-      </c>
-      <c r="U22" s="58">
-        <v>0</v>
-      </c>
-      <c r="V22" s="57">
+      <c r="B22" s="51">
+        <v>0</v>
+      </c>
+      <c r="C22" s="44">
+        <v>0</v>
+      </c>
+      <c r="D22" s="44">
+        <v>0</v>
+      </c>
+      <c r="E22" s="44">
+        <v>0</v>
+      </c>
+      <c r="F22" s="51">
+        <v>0</v>
+      </c>
+      <c r="G22" s="51">
+        <v>0</v>
+      </c>
+      <c r="H22" s="51">
+        <v>0</v>
+      </c>
+      <c r="I22" s="44">
+        <v>0</v>
+      </c>
+      <c r="J22" s="44">
+        <v>0</v>
+      </c>
+      <c r="K22" s="44">
+        <v>0</v>
+      </c>
+      <c r="L22" s="44">
+        <v>0</v>
+      </c>
+      <c r="M22" s="44">
+        <v>0</v>
+      </c>
+      <c r="N22" s="44">
+        <v>0</v>
+      </c>
+      <c r="O22" s="51">
+        <v>0</v>
+      </c>
+      <c r="P22" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="44">
+        <v>0</v>
+      </c>
+      <c r="R22" s="44">
+        <v>0</v>
+      </c>
+      <c r="S22" s="44">
+        <v>0</v>
+      </c>
+      <c r="T22" s="44">
+        <v>0</v>
+      </c>
+      <c r="U22" s="44">
+        <v>0</v>
+      </c>
+      <c r="V22" s="52">
         <f>'Data from BFPIaE'!E25/'Data from BFPIaE'!C25</f>
         <v>0</v>
       </c>
       <c r="W22" s="7"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -3922,8 +3916,8 @@
       <c r="V23" s="44"/>
       <c r="W23" s="7"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A25" s="63"/>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3931,12 +3925,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4169,29 +4165,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E00F3CCD-FB36-47C2-88EB-9171D0759985}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F47E5E3D-FA85-4869-B130-7195F7099568}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3BF454-BC11-4F6C-A469-2988498C51EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4200,4 +4182,31 @@
     <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F47E5E3D-FA85-4869-B130-7195F7099568}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E00F3CCD-FB36-47C2-88EB-9171D0759985}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Set all crude oil export drivers to zero in PoFDCtAE
</commit_message>
<xml_diff>
--- a/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
+++ b/InputData/fuels/PoFDCtAE/Perc of Fuel Demand Changes that Affect Exports.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rachel Goldstein\Dropbox (Energy Innovation)\Desktop\Vensim files from GitHub\EPS EU\InputData\fuels\PoFDCtAE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu\InputData\fuels\PoFDCtAE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986ACDB5-CA33-45D5-8BAC-E4180D35192C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC074563-BCAA-4EBD-A12A-293DBEA0BF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="1170" windowWidth="30990" windowHeight="12645" activeTab="2" xr2:uid="{3E0B3505-0335-466F-B5FC-C5183A2DB44F}"/>
+    <workbookView xWindow="32085" yWindow="3945" windowWidth="21585" windowHeight="12525" activeTab="1" xr2:uid="{3E0B3505-0335-466F-B5FC-C5183A2DB44F}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -193,9 +193,6 @@
     <t>day exports / present day production) are used, which should roughly express how important the export market</t>
   </si>
   <si>
-    <t>The same assumptions are chosen for the EU.</t>
-  </si>
-  <si>
     <t>Start Year Data from BFPIaE</t>
   </si>
   <si>
@@ -307,9 +304,6 @@
     <t>Start Year Production, Imports and Exports</t>
   </si>
   <si>
-    <t>The start year taken in this model in 2021</t>
-  </si>
-  <si>
     <t>The estimation of the response to a drop in domestic use of a secondary petroleum product is done by observing how large</t>
   </si>
   <si>
@@ -326,6 +320,12 @@
   </si>
   <si>
     <t>BAU Fuel Production Imports and Exports (BFPIaE) Variable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We alter these assumptions for the EU, which exports very little oil and gas. </t>
+  </si>
+  <si>
+    <t>The start year taken in this model in 2022</t>
   </si>
 </sst>
 </file>
@@ -668,14 +668,14 @@
     <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1109,369 +1109,369 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937B2E0C-144E-4608-927D-ACF1F00D1421}">
   <dimension ref="B10:D90"/>
   <sheetViews>
-    <sheetView topLeftCell="B34" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView topLeftCell="B52" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="10.85546875" style="2"/>
-    <col min="3" max="3" width="44.28515625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.85546875" style="2"/>
+    <col min="1" max="2" width="10.81640625" style="2"/>
+    <col min="3" max="3" width="44.26953125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="10.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C16" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B19" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B20" s="6"/>
       <c r="C20" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B21" s="6"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C22" s="45" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C23" s="45" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C24" s="45"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C25" s="45" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C26" s="45" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C27" s="45" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C28" s="45" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C29" s="45" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C30" s="45" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C31" s="45" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C32" s="45" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C33" s="45"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C34" s="45" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C35" s="45"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C36" s="45" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C37" s="45"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C38" s="46" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C39" s="45" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C40" s="45" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C41" s="45" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C42" s="45" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C43" s="45" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C44" s="45" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C45" s="45" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C46" s="45" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C47" s="45" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C48" s="45"/>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C49" s="47" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C50" s="45" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C51" s="45" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C52" s="45" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C53" s="45" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C54" s="45"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C55" s="45" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C56" s="45" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C57" s="45" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C58" s="45"/>
     </row>
-    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C59" s="45" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C60" s="45"/>
     </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C61" s="47" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C62" s="45" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C63" s="45" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C64" s="45" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C65" s="45" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C66" s="45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C67" s="45" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C68" s="45"/>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C69" s="45" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C70" s="45" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C71" s="45" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C72" s="45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C73" s="45" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C74" s="45" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C75" s="45"/>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C76" s="45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C77" s="45" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C78" s="45" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B79" s="5"/>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B80" s="5"/>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B81" s="5"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B82" s="5"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B83" s="5"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B84" s="5"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B85" s="5"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B86" s="5"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B87" s="5"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B88" s="5"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B89" s="5"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B90" s="5"/>
     </row>
   </sheetData>
@@ -1484,51 +1484,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11FBB9C7-1AAD-4CCB-BFB3-78988F2C384F}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="59"/>
+      <c r="B1" s="59"/>
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
       <c r="J1" s="7"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
+      <c r="K1" s="59"/>
+      <c r="L1" s="59"/>
       <c r="M1" s="7"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="7"/>
       <c r="B2" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
       <c r="F2" s="9"/>
       <c r="G2" s="10"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="57"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="59"/>
       <c r="J2" s="7"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="7"/>
       <c r="B3" s="11" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -1536,53 +1536,53 @@
       <c r="F3" s="12"/>
       <c r="G3" s="13"/>
       <c r="H3" s="7"/>
-      <c r="I3" s="59" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="60"/>
+      <c r="I3" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" s="58"/>
       <c r="K3" s="7"/>
       <c r="L3" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>
       <c r="B4" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="F4" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="18" t="s">
         <v>59</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>60</v>
       </c>
       <c r="H4" s="7"/>
       <c r="I4" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="20" t="s">
         <v>58</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>59</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="22"/>
@@ -1594,14 +1594,14 @@
       <c r="J5" s="23"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C6" s="26">
         <v>1316013899314200</v>
@@ -1617,7 +1617,7 @@
         <v>3773221967618100</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="29">
@@ -1630,14 +1630,14 @@
       </c>
       <c r="K6" s="7"/>
       <c r="L6" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="7"/>
       <c r="B7" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C7" s="26">
         <v>1506541668893400</v>
@@ -1653,7 +1653,7 @@
         <v>1.27693348242714E+16</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H7" s="7"/>
       <c r="I7" s="29">
@@ -1666,14 +1666,14 @@
       </c>
       <c r="K7" s="7"/>
       <c r="L7" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="7"/>
       <c r="B8" s="25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" s="26">
         <v>12298119600000</v>
@@ -1689,7 +1689,7 @@
         <v>8742645600000000</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H8" s="7"/>
       <c r="I8" s="29">
@@ -1702,14 +1702,14 @@
       </c>
       <c r="K8" s="7"/>
       <c r="L8" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="7"/>
       <c r="B9" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="22"/>
@@ -1721,14 +1721,14 @@
       <c r="J9" s="41"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="7"/>
       <c r="B10" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
@@ -1738,14 +1738,14 @@
       <c r="H10" s="7"/>
       <c r="I10" s="40"/>
       <c r="J10" s="41"/>
-      <c r="K10" s="58"/>
-      <c r="L10" s="57"/>
+      <c r="K10" s="60"/>
+      <c r="L10" s="59"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="7"/>
       <c r="B11" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="22"/>
@@ -1755,14 +1755,14 @@
       <c r="H11" s="7"/>
       <c r="I11" s="40"/>
       <c r="J11" s="41"/>
-      <c r="K11" s="58"/>
-      <c r="L11" s="57"/>
+      <c r="K11" s="60"/>
+      <c r="L11" s="59"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="7"/>
       <c r="B12" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C12" s="26">
         <v>4604009174358300</v>
@@ -1778,7 +1778,7 @@
         <v>4774280903958000</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H12" s="7"/>
       <c r="I12" s="29">
@@ -1789,14 +1789,14 @@
         <f t="shared" si="1"/>
         <v>0.95507604016524161</v>
       </c>
-      <c r="K12" s="58"/>
-      <c r="L12" s="57"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="59"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="7"/>
       <c r="B13" s="32" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="26">
         <v>3846173394503100</v>
@@ -1812,7 +1812,7 @@
         <v>1871712777417600</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="42">
@@ -1823,14 +1823,14 @@
         <f t="shared" si="1"/>
         <v>0.3922833651703625</v>
       </c>
-      <c r="K13" s="58"/>
-      <c r="L13" s="57"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="59"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="7"/>
       <c r="B14" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C14" s="26">
         <v>8698175395867500</v>
@@ -1846,7 +1846,7 @@
         <v>9225920109422400</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="42">
@@ -1857,14 +1857,14 @@
         <f t="shared" si="1"/>
         <v>0.70550484210364817</v>
       </c>
-      <c r="K14" s="58"/>
-      <c r="L14" s="57"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="59"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="7"/>
       <c r="B15" s="25" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C15" s="26">
         <v>95936235552900</v>
@@ -1880,7 +1880,7 @@
         <v>124792000133400</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H15" s="7"/>
       <c r="I15" s="29">
@@ -1891,14 +1891,14 @@
         <f t="shared" si="1"/>
         <v>0.71852702501386922</v>
       </c>
-      <c r="K15" s="58"/>
-      <c r="L15" s="57"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="59"/>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="7"/>
       <c r="B16" s="25" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C16" s="26">
         <v>509765927952000</v>
@@ -1914,7 +1914,7 @@
         <v>570359521616700</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H16" s="7"/>
       <c r="I16" s="29">
@@ -1925,14 +1925,14 @@
         <f t="shared" si="1"/>
         <v>0.62841900526223626</v>
       </c>
-      <c r="K16" s="58"/>
-      <c r="L16" s="57"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="59"/>
       <c r="M16" s="7"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="7"/>
       <c r="B17" s="32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C17" s="26">
         <v>2655840079297500</v>
@@ -1948,7 +1948,7 @@
         <v>3898553142031200</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="42">
@@ -1959,14 +1959,14 @@
         <f t="shared" si="1"/>
         <v>0.72086022686964368</v>
       </c>
-      <c r="K17" s="58"/>
-      <c r="L17" s="57"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="59"/>
       <c r="M17" s="7"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="7"/>
       <c r="B18" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
@@ -1976,14 +1976,14 @@
       <c r="H18" s="7"/>
       <c r="I18" s="40"/>
       <c r="J18" s="41"/>
-      <c r="K18" s="58"/>
-      <c r="L18" s="57"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="59"/>
       <c r="M18" s="7"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="7"/>
       <c r="B19" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" s="22"/>
       <c r="D19" s="22"/>
@@ -1993,14 +1993,14 @@
       <c r="H19" s="7"/>
       <c r="I19" s="40"/>
       <c r="J19" s="41"/>
-      <c r="K19" s="58"/>
-      <c r="L19" s="57"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="59"/>
       <c r="M19" s="7"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="7"/>
       <c r="B20" s="25" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C20" s="26">
         <v>2311596409121700</v>
@@ -2016,7 +2016,7 @@
         <v>2274792794223900</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H20" s="7"/>
       <c r="I20" s="29">
@@ -2027,14 +2027,14 @@
         <f t="shared" si="1"/>
         <v>0.8807194770978013</v>
       </c>
-      <c r="K20" s="58"/>
-      <c r="L20" s="57"/>
+      <c r="K20" s="60"/>
+      <c r="L20" s="59"/>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="7"/>
       <c r="B21" s="25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C21" s="26">
         <v>815168414777399.88</v>
@@ -2050,7 +2050,7 @@
         <v>1.88591423984418E+16</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="29">
@@ -2061,14 +2061,14 @@
         <f t="shared" si="1"/>
         <v>0.99453702179044434</v>
       </c>
-      <c r="K21" s="58"/>
-      <c r="L21" s="57"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="59"/>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="7"/>
       <c r="B22" s="32" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C22" s="26">
         <v>4205419459049399.5</v>
@@ -2084,7 +2084,7 @@
         <v>4035986709549900</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H22" s="7"/>
       <c r="I22" s="42">
@@ -2095,14 +2095,14 @@
         <f t="shared" si="1"/>
         <v>0.49856575142985632</v>
       </c>
-      <c r="K22" s="58"/>
-      <c r="L22" s="57"/>
+      <c r="K22" s="60"/>
+      <c r="L22" s="59"/>
       <c r="M22" s="7"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
       <c r="B23" s="32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C23" s="26">
         <v>1351107251968200.3</v>
@@ -2118,7 +2118,7 @@
         <v>1893265423006500</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="42">
@@ -2129,14 +2129,14 @@
         <f t="shared" si="1"/>
         <v>0.84498067686633227</v>
       </c>
-      <c r="K23" s="58"/>
-      <c r="L23" s="57"/>
+      <c r="K23" s="60"/>
+      <c r="L23" s="59"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="7"/>
       <c r="B24" s="25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="33">
         <v>921931628601900.13</v>
@@ -2152,7 +2152,7 @@
         <v>963082050907500.13</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="29">
@@ -2163,14 +2163,14 @@
         <f t="shared" si="1"/>
         <v>0.9981760467937546</v>
       </c>
-      <c r="K24" s="58"/>
-      <c r="L24" s="57"/>
+      <c r="K24" s="60"/>
+      <c r="L24" s="59"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="7"/>
       <c r="B25" s="34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C25" s="35">
         <v>15079578000</v>
@@ -2186,7 +2186,7 @@
         <v>15079578000</v>
       </c>
       <c r="G25" s="37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H25" s="7"/>
       <c r="I25" s="29">
@@ -2197,95 +2197,107 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K25" s="58"/>
-      <c r="L25" s="57"/>
+      <c r="K25" s="60"/>
+      <c r="L25" s="59"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="57"/>
-      <c r="B26" s="57"/>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="59"/>
+      <c r="B26" s="59"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
       <c r="J26" s="7"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="59"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="57"/>
-      <c r="B27" s="57"/>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="59"/>
+      <c r="B27" s="59"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="57"/>
-      <c r="I27" s="57"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="59"/>
       <c r="J27" s="7"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="57"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="7"/>
       <c r="B28" s="38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C28" s="39"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
-      <c r="H28" s="57"/>
-      <c r="I28" s="57"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
       <c r="J28" s="7"/>
-      <c r="K28" s="57"/>
-      <c r="L28" s="57"/>
+      <c r="K28" s="59"/>
+      <c r="L28" s="59"/>
       <c r="M28" s="7"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="57"/>
-      <c r="B29" s="57"/>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="59"/>
+      <c r="B29" s="59"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="57"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="59"/>
       <c r="J29" s="7"/>
-      <c r="K29" s="57"/>
-      <c r="L29" s="57"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="59"/>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="57"/>
-      <c r="B30" s="57"/>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" s="59"/>
+      <c r="B30" s="59"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="57"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="59"/>
       <c r="J30" s="7"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
+      <c r="K30" s="59"/>
+      <c r="L30" s="59"/>
       <c r="M30" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="K30:L30"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="K28:L28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="K24:L24"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="K26:L26"/>
     <mergeCell ref="K21:L21"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="K11:L11"/>
@@ -2298,24 +2310,12 @@
     <mergeCell ref="K18:L18"/>
     <mergeCell ref="K19:L19"/>
     <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="K24:L24"/>
-    <mergeCell ref="K25:L25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="K30:L30"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="K28:L28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="K29:L29"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="K2:L2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2328,105 +2328,105 @@
   </sheetPr>
   <dimension ref="A1:W25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R18" sqref="R18"/>
+      <selection pane="bottomRight" activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="48" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="50" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D1" s="50" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F1" s="49" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G1" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="I1" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="J1" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="K1" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="50" t="s">
+      <c r="L1" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="L1" s="50" t="s">
+      <c r="M1" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="N1" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="N1" s="50" t="s">
+      <c r="O1" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="O1" s="49" t="s">
+      <c r="P1" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="49" t="s">
+      <c r="Q1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="Q1" s="50" t="s">
+      <c r="R1" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="R1" s="50" t="s">
+      <c r="S1" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="S1" s="50" t="s">
+      <c r="T1" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="T1" s="50" t="s">
+      <c r="U1" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="U1" s="50" t="s">
+      <c r="V1" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="V1" s="50" t="s">
-        <v>85</v>
-      </c>
       <c r="W1" s="7"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" s="51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="51">
         <v>0</v>
@@ -2493,9 +2493,9 @@
       </c>
       <c r="W2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="51">
         <v>0</v>
@@ -2563,9 +2563,9 @@
       </c>
       <c r="W3" s="7"/>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" s="51">
         <v>0</v>
@@ -2632,9 +2632,9 @@
       </c>
       <c r="W4" s="7"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B5" s="51">
         <v>0</v>
@@ -2702,9 +2702,9 @@
       </c>
       <c r="W5" s="7"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B6" s="51">
         <v>0</v>
@@ -2771,147 +2771,147 @@
       </c>
       <c r="W6" s="7"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="51">
+        <v>0</v>
+      </c>
+      <c r="C7" s="51">
+        <v>0</v>
+      </c>
+      <c r="D7" s="51">
+        <v>0</v>
+      </c>
+      <c r="E7" s="51">
+        <v>0</v>
+      </c>
+      <c r="F7" s="51">
+        <v>0</v>
+      </c>
+      <c r="G7" s="51">
+        <v>0</v>
+      </c>
+      <c r="H7" s="51">
+        <v>0</v>
+      </c>
+      <c r="I7" s="51">
+        <v>0</v>
+      </c>
+      <c r="J7" s="51">
+        <v>0</v>
+      </c>
+      <c r="K7" s="51">
+        <v>0</v>
+      </c>
+      <c r="L7" s="51">
+        <v>0</v>
+      </c>
+      <c r="M7" s="51">
+        <v>0</v>
+      </c>
+      <c r="N7" s="51">
+        <v>0</v>
+      </c>
+      <c r="O7" s="51">
+        <v>0</v>
+      </c>
+      <c r="P7" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="51">
+        <v>0</v>
+      </c>
+      <c r="R7" s="51">
+        <v>0</v>
+      </c>
+      <c r="S7" s="51">
+        <v>0</v>
+      </c>
+      <c r="T7" s="51">
+        <v>0</v>
+      </c>
+      <c r="U7" s="51">
+        <v>0</v>
+      </c>
+      <c r="V7" s="51">
+        <v>0</v>
+      </c>
+      <c r="W7" s="7"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="51">
-        <v>0</v>
-      </c>
-      <c r="C7" s="51">
-        <v>0</v>
-      </c>
-      <c r="D7" s="51">
-        <v>0</v>
-      </c>
-      <c r="E7" s="51">
-        <v>0</v>
-      </c>
-      <c r="F7" s="51">
-        <v>0</v>
-      </c>
-      <c r="G7" s="51">
-        <v>0</v>
-      </c>
-      <c r="H7" s="51">
-        <v>0</v>
-      </c>
-      <c r="I7" s="51">
-        <v>0</v>
-      </c>
-      <c r="J7" s="51">
-        <v>0</v>
-      </c>
-      <c r="K7" s="51">
-        <v>0</v>
-      </c>
-      <c r="L7" s="51">
-        <v>0</v>
-      </c>
-      <c r="M7" s="51">
-        <v>0</v>
-      </c>
-      <c r="N7" s="51">
-        <v>0</v>
-      </c>
-      <c r="O7" s="51">
-        <v>0</v>
-      </c>
-      <c r="P7" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="51">
-        <v>0</v>
-      </c>
-      <c r="R7" s="51">
-        <v>0</v>
-      </c>
-      <c r="S7" s="51">
-        <v>0</v>
-      </c>
-      <c r="T7" s="51">
-        <v>0</v>
-      </c>
-      <c r="U7" s="51">
-        <v>0</v>
-      </c>
-      <c r="V7" s="51">
-        <v>0</v>
-      </c>
-      <c r="W7" s="7"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="B8" s="51">
+        <v>0</v>
+      </c>
+      <c r="C8" s="51">
+        <v>0</v>
+      </c>
+      <c r="D8" s="51">
+        <v>0</v>
+      </c>
+      <c r="E8" s="51">
+        <v>0</v>
+      </c>
+      <c r="F8" s="51">
+        <v>0</v>
+      </c>
+      <c r="G8" s="51">
+        <v>0</v>
+      </c>
+      <c r="H8" s="51">
+        <v>0</v>
+      </c>
+      <c r="I8" s="51">
+        <v>0</v>
+      </c>
+      <c r="J8" s="51">
+        <v>0</v>
+      </c>
+      <c r="K8" s="51">
+        <v>0</v>
+      </c>
+      <c r="L8" s="51">
+        <v>0</v>
+      </c>
+      <c r="M8" s="51">
+        <v>0</v>
+      </c>
+      <c r="N8" s="51">
+        <v>0</v>
+      </c>
+      <c r="O8" s="51">
+        <v>0</v>
+      </c>
+      <c r="P8" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="51">
+        <v>0</v>
+      </c>
+      <c r="R8" s="51">
+        <v>0</v>
+      </c>
+      <c r="S8" s="51">
+        <v>0</v>
+      </c>
+      <c r="T8" s="51">
+        <v>0</v>
+      </c>
+      <c r="U8" s="51">
+        <v>0</v>
+      </c>
+      <c r="V8" s="51">
+        <v>0</v>
+      </c>
+      <c r="W8" s="7"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="B8" s="51">
-        <v>0</v>
-      </c>
-      <c r="C8" s="51">
-        <v>0</v>
-      </c>
-      <c r="D8" s="51">
-        <v>0</v>
-      </c>
-      <c r="E8" s="51">
-        <v>0</v>
-      </c>
-      <c r="F8" s="51">
-        <v>0</v>
-      </c>
-      <c r="G8" s="51">
-        <v>0</v>
-      </c>
-      <c r="H8" s="51">
-        <v>0</v>
-      </c>
-      <c r="I8" s="51">
-        <v>0</v>
-      </c>
-      <c r="J8" s="51">
-        <v>0</v>
-      </c>
-      <c r="K8" s="51">
-        <v>0</v>
-      </c>
-      <c r="L8" s="51">
-        <v>0</v>
-      </c>
-      <c r="M8" s="51">
-        <v>0</v>
-      </c>
-      <c r="N8" s="51">
-        <v>0</v>
-      </c>
-      <c r="O8" s="51">
-        <v>0</v>
-      </c>
-      <c r="P8" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="51">
-        <v>0</v>
-      </c>
-      <c r="R8" s="51">
-        <v>0</v>
-      </c>
-      <c r="S8" s="51">
-        <v>0</v>
-      </c>
-      <c r="T8" s="51">
-        <v>0</v>
-      </c>
-      <c r="U8" s="51">
-        <v>0</v>
-      </c>
-      <c r="V8" s="51">
-        <v>0</v>
-      </c>
-      <c r="W8" s="7"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="B9" s="51">
         <v>0</v>
@@ -2979,9 +2979,9 @@
       </c>
       <c r="W9" s="7"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B10" s="51">
         <v>0</v>
@@ -3033,8 +3033,7 @@
         <v>0</v>
       </c>
       <c r="R10" s="55">
-        <f>1-J10</f>
-        <v>0.39228336517036244</v>
+        <v>0</v>
       </c>
       <c r="S10" s="44">
         <v>0</v>
@@ -3050,9 +3049,9 @@
       </c>
       <c r="W10" s="7"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="51">
         <v>0</v>
@@ -3104,8 +3103,7 @@
         <v>0</v>
       </c>
       <c r="R11" s="55">
-        <f>1-K11</f>
-        <v>0.70550484210364806</v>
+        <v>0</v>
       </c>
       <c r="S11" s="44">
         <v>0</v>
@@ -3121,9 +3119,9 @@
       </c>
       <c r="W11" s="7"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" s="51">
         <v>0</v>
@@ -3191,9 +3189,9 @@
       </c>
       <c r="W12" s="7"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B13" s="51">
         <v>0</v>
@@ -3261,9 +3259,9 @@
       </c>
       <c r="W13" s="7"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" s="51">
         <v>0</v>
@@ -3315,8 +3313,7 @@
         <v>0</v>
       </c>
       <c r="R14" s="55">
-        <f>1-N14</f>
-        <v>0.72086022686964368</v>
+        <v>0</v>
       </c>
       <c r="S14" s="44">
         <v>0</v>
@@ -3332,147 +3329,147 @@
       </c>
       <c r="W14" s="7"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A15" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="51">
+        <v>0</v>
+      </c>
+      <c r="C15" s="51">
+        <v>0</v>
+      </c>
+      <c r="D15" s="51">
+        <v>0</v>
+      </c>
+      <c r="E15" s="51">
+        <v>0</v>
+      </c>
+      <c r="F15" s="51">
+        <v>0</v>
+      </c>
+      <c r="G15" s="51">
+        <v>0</v>
+      </c>
+      <c r="H15" s="51">
+        <v>0</v>
+      </c>
+      <c r="I15" s="51">
+        <v>0</v>
+      </c>
+      <c r="J15" s="51">
+        <v>0</v>
+      </c>
+      <c r="K15" s="51">
+        <v>0</v>
+      </c>
+      <c r="L15" s="51">
+        <v>0</v>
+      </c>
+      <c r="M15" s="51">
+        <v>0</v>
+      </c>
+      <c r="N15" s="51">
+        <v>0</v>
+      </c>
+      <c r="O15" s="51">
+        <v>0</v>
+      </c>
+      <c r="P15" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="51">
+        <v>0</v>
+      </c>
+      <c r="R15" s="51">
+        <v>0</v>
+      </c>
+      <c r="S15" s="51">
+        <v>0</v>
+      </c>
+      <c r="T15" s="51">
+        <v>0</v>
+      </c>
+      <c r="U15" s="51">
+        <v>0</v>
+      </c>
+      <c r="V15" s="51">
+        <v>0</v>
+      </c>
+      <c r="W15" s="7"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A16" s="53" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="51">
-        <v>0</v>
-      </c>
-      <c r="C15" s="51">
-        <v>0</v>
-      </c>
-      <c r="D15" s="51">
-        <v>0</v>
-      </c>
-      <c r="E15" s="51">
-        <v>0</v>
-      </c>
-      <c r="F15" s="51">
-        <v>0</v>
-      </c>
-      <c r="G15" s="51">
-        <v>0</v>
-      </c>
-      <c r="H15" s="51">
-        <v>0</v>
-      </c>
-      <c r="I15" s="51">
-        <v>0</v>
-      </c>
-      <c r="J15" s="51">
-        <v>0</v>
-      </c>
-      <c r="K15" s="51">
-        <v>0</v>
-      </c>
-      <c r="L15" s="51">
-        <v>0</v>
-      </c>
-      <c r="M15" s="51">
-        <v>0</v>
-      </c>
-      <c r="N15" s="51">
-        <v>0</v>
-      </c>
-      <c r="O15" s="51">
-        <v>0</v>
-      </c>
-      <c r="P15" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="51">
-        <v>0</v>
-      </c>
-      <c r="R15" s="51">
-        <v>0</v>
-      </c>
-      <c r="S15" s="51">
-        <v>0</v>
-      </c>
-      <c r="T15" s="51">
-        <v>0</v>
-      </c>
-      <c r="U15" s="51">
-        <v>0</v>
-      </c>
-      <c r="V15" s="51">
-        <v>0</v>
-      </c>
-      <c r="W15" s="7"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
+      <c r="B16" s="51">
+        <v>0</v>
+      </c>
+      <c r="C16" s="51">
+        <v>0</v>
+      </c>
+      <c r="D16" s="51">
+        <v>0</v>
+      </c>
+      <c r="E16" s="51">
+        <v>0</v>
+      </c>
+      <c r="F16" s="51">
+        <v>0</v>
+      </c>
+      <c r="G16" s="51">
+        <v>0</v>
+      </c>
+      <c r="H16" s="51">
+        <v>0</v>
+      </c>
+      <c r="I16" s="51">
+        <v>0</v>
+      </c>
+      <c r="J16" s="51">
+        <v>0</v>
+      </c>
+      <c r="K16" s="51">
+        <v>0</v>
+      </c>
+      <c r="L16" s="51">
+        <v>0</v>
+      </c>
+      <c r="M16" s="51">
+        <v>0</v>
+      </c>
+      <c r="N16" s="51">
+        <v>0</v>
+      </c>
+      <c r="O16" s="51">
+        <v>0</v>
+      </c>
+      <c r="P16" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="51">
+        <v>0</v>
+      </c>
+      <c r="R16" s="51">
+        <v>0</v>
+      </c>
+      <c r="S16" s="51">
+        <v>0</v>
+      </c>
+      <c r="T16" s="51">
+        <v>0</v>
+      </c>
+      <c r="U16" s="51">
+        <v>0</v>
+      </c>
+      <c r="V16" s="51">
+        <v>0</v>
+      </c>
+      <c r="W16" s="7"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="B16" s="51">
-        <v>0</v>
-      </c>
-      <c r="C16" s="51">
-        <v>0</v>
-      </c>
-      <c r="D16" s="51">
-        <v>0</v>
-      </c>
-      <c r="E16" s="51">
-        <v>0</v>
-      </c>
-      <c r="F16" s="51">
-        <v>0</v>
-      </c>
-      <c r="G16" s="51">
-        <v>0</v>
-      </c>
-      <c r="H16" s="51">
-        <v>0</v>
-      </c>
-      <c r="I16" s="51">
-        <v>0</v>
-      </c>
-      <c r="J16" s="51">
-        <v>0</v>
-      </c>
-      <c r="K16" s="51">
-        <v>0</v>
-      </c>
-      <c r="L16" s="51">
-        <v>0</v>
-      </c>
-      <c r="M16" s="51">
-        <v>0</v>
-      </c>
-      <c r="N16" s="51">
-        <v>0</v>
-      </c>
-      <c r="O16" s="51">
-        <v>0</v>
-      </c>
-      <c r="P16" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="51">
-        <v>0</v>
-      </c>
-      <c r="R16" s="51">
-        <v>0</v>
-      </c>
-      <c r="S16" s="51">
-        <v>0</v>
-      </c>
-      <c r="T16" s="51">
-        <v>0</v>
-      </c>
-      <c r="U16" s="51">
-        <v>0</v>
-      </c>
-      <c r="V16" s="51">
-        <v>0</v>
-      </c>
-      <c r="W16" s="7"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="B17" s="51">
         <v>0</v>
@@ -3540,79 +3537,79 @@
       </c>
       <c r="W17" s="7"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A18" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="51">
+        <v>0</v>
+      </c>
+      <c r="C18" s="44">
+        <v>0</v>
+      </c>
+      <c r="D18" s="44">
+        <v>0</v>
+      </c>
+      <c r="E18" s="44">
+        <v>0</v>
+      </c>
+      <c r="F18" s="51">
+        <v>0</v>
+      </c>
+      <c r="G18" s="51">
+        <v>0</v>
+      </c>
+      <c r="H18" s="51">
+        <v>0</v>
+      </c>
+      <c r="I18" s="44">
+        <v>0</v>
+      </c>
+      <c r="J18" s="44">
+        <v>0</v>
+      </c>
+      <c r="K18" s="44">
+        <v>0</v>
+      </c>
+      <c r="L18" s="44">
+        <v>0</v>
+      </c>
+      <c r="M18" s="44">
+        <v>0</v>
+      </c>
+      <c r="N18" s="44">
+        <v>0</v>
+      </c>
+      <c r="O18" s="51">
+        <v>0</v>
+      </c>
+      <c r="P18" s="51">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="44">
+        <v>0</v>
+      </c>
+      <c r="R18" s="54">
+        <v>0</v>
+      </c>
+      <c r="S18" s="44">
+        <v>0</v>
+      </c>
+      <c r="T18" s="44">
+        <v>0</v>
+      </c>
+      <c r="U18" s="44">
+        <v>0</v>
+      </c>
+      <c r="V18" s="44">
+        <v>0</v>
+      </c>
+      <c r="W18" s="7"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="51">
-        <v>0</v>
-      </c>
-      <c r="C18" s="44">
-        <v>0</v>
-      </c>
-      <c r="D18" s="44">
-        <v>0</v>
-      </c>
-      <c r="E18" s="44">
-        <v>0</v>
-      </c>
-      <c r="F18" s="51">
-        <v>0</v>
-      </c>
-      <c r="G18" s="51">
-        <v>0</v>
-      </c>
-      <c r="H18" s="51">
-        <v>0</v>
-      </c>
-      <c r="I18" s="44">
-        <v>0</v>
-      </c>
-      <c r="J18" s="44">
-        <v>0</v>
-      </c>
-      <c r="K18" s="44">
-        <v>0</v>
-      </c>
-      <c r="L18" s="44">
-        <v>0</v>
-      </c>
-      <c r="M18" s="44">
-        <v>0</v>
-      </c>
-      <c r="N18" s="44">
-        <v>0</v>
-      </c>
-      <c r="O18" s="51">
-        <v>0</v>
-      </c>
-      <c r="P18" s="51">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="44">
-        <v>0</v>
-      </c>
-      <c r="R18" s="54">
-        <v>0</v>
-      </c>
-      <c r="S18" s="44">
-        <v>0</v>
-      </c>
-      <c r="T18" s="44">
-        <v>0</v>
-      </c>
-      <c r="U18" s="44">
-        <v>0</v>
-      </c>
-      <c r="V18" s="44">
-        <v>0</v>
-      </c>
-      <c r="W18" s="7"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>82</v>
-      </c>
       <c r="B19" s="51">
         <v>0</v>
       </c>
@@ -3662,8 +3659,7 @@
         <v>0</v>
       </c>
       <c r="R19" s="55">
-        <f>1-S19</f>
-        <v>0.49856575142985637</v>
+        <v>0</v>
       </c>
       <c r="S19" s="54">
         <f>'Data from BFPIaE'!E22/SUM('Data from BFPIaE'!E22:F22)</f>
@@ -3680,9 +3676,9 @@
       </c>
       <c r="W19" s="7"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" s="51">
         <v>0</v>
@@ -3733,8 +3729,7 @@
         <v>0</v>
       </c>
       <c r="R20" s="55">
-        <f>1-T20</f>
-        <v>0.84498067686633227</v>
+        <v>0</v>
       </c>
       <c r="S20" s="44">
         <v>0</v>
@@ -3751,9 +3746,9 @@
       </c>
       <c r="W20" s="7"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B21" s="51">
         <v>0</v>
@@ -3821,9 +3816,9 @@
       </c>
       <c r="W21" s="7"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="51">
         <v>0</v>
@@ -3891,7 +3886,7 @@
       </c>
       <c r="W22" s="7"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A23" s="7"/>
       <c r="B23" s="44"/>
       <c r="C23" s="44"/>
@@ -3916,7 +3911,7 @@
       <c r="V23" s="44"/>
       <c r="W23" s="7"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="39"/>
     </row>
   </sheetData>
@@ -3925,14 +3920,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4165,21 +4158,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="00484652-42e1-479e-92f4-fb0efddcdf60">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3BF454-BC11-4F6C-A469-2988498C51EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E00F3CCD-FB36-47C2-88EB-9171D0759985}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
-    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4204,9 +4196,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E00F3CCD-FB36-47C2-88EB-9171D0759985}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3BF454-BC11-4F6C-A469-2988498C51EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="00484652-42e1-479e-92f4-fb0efddcdf60"/>
+    <ds:schemaRef ds:uri="41b1c9bf-5b6b-463b-ba12-a3b9bfbff0d3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>